<commit_message>
updating hardest games to show home/away/neutral
</commit_message>
<xml_diff>
--- a/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week1.xlsx
+++ b/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M94"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1239,34 +1239,34 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Wake Forest</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>App State</t>
+          <t>Kennesaw State</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>4.4</v>
+        <v>5.100000000000001</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>App State -8.5</t>
+          <t>Wake Forest -17.5</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>App State -8.5</t>
+          <t>Wake Forest -17.5</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>App State -12.9</t>
+          <t>Wake Forest -22.6</t>
         </is>
       </c>
       <c r="H20" t="n">
-        <v>-8.5</v>
+        <v>17.5</v>
       </c>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
@@ -1280,12 +1280,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Notre Dame</t>
+          <t>App State</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -1293,21 +1293,21 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Notre Dame -2.5</t>
+          <t>App State -8.5</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Notre Dame -2.5</t>
+          <t>App State -8.5</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Notre Dame -6.9</t>
+          <t>App State -12.9</t>
         </is>
       </c>
       <c r="H21" t="n">
-        <v>-2.5</v>
+        <v>-8.5</v>
       </c>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
@@ -1321,34 +1321,34 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>North Carolina</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>TCU</t>
+          <t>Notre Dame</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>4.2</v>
+        <v>4.4</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>TCU -3.0</t>
+          <t>Notre Dame -2.5</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>TCU -3</t>
+          <t>Notre Dame -2.5</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>TCU -7.2</t>
+          <t>Notre Dame -6.9</t>
         </is>
       </c>
       <c r="H22" t="n">
-        <v>-3</v>
+        <v>-2.5</v>
       </c>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
@@ -1362,34 +1362,34 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Syracuse</t>
+          <t>North Carolina</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Tennessee</t>
+          <t>TCU</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>4.100000000000001</v>
+        <v>4.2</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Tennessee -13.5</t>
+          <t>TCU -3.0</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Tennessee -13.5</t>
+          <t>TCU -3</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Tennessee -17.6</t>
+          <t>TCU -7.2</t>
         </is>
       </c>
       <c r="H23" t="n">
-        <v>-13.5</v>
+        <v>-3</v>
       </c>
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
@@ -1403,34 +1403,34 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Massachusetts</t>
+          <t>Syracuse</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Temple</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>3.9</v>
+        <v>4.100000000000001</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Temple -3.0</t>
+          <t>Tennessee -13.5</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Temple -3</t>
+          <t>Tennessee -13.5</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Massachusetts -0.9</t>
+          <t>Tennessee -17.6</t>
         </is>
       </c>
       <c r="H24" t="n">
-        <v>-3</v>
+        <v>-13.5</v>
       </c>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
@@ -1444,34 +1444,34 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Michigan</t>
+          <t>Massachusetts</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>New Mexico</t>
+          <t>Temple</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>3.899999999999999</v>
+        <v>3.9</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Michigan -36.5</t>
+          <t>Temple -3.0</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Michigan -36.5</t>
+          <t>Temple -3</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Michigan -40.4</t>
+          <t>Massachusetts -0.9</t>
         </is>
       </c>
       <c r="H25" t="n">
-        <v>36.5</v>
+        <v>-3</v>
       </c>
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
@@ -1485,34 +1485,34 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Hawai'i</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Stanford</t>
+          <t>New Mexico</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>3.8</v>
+        <v>3.899999999999999</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Hawai'i -1.5</t>
+          <t>Michigan -36.5</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Hawai'i -1.5</t>
+          <t>Michigan -36.5</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Stanford -2.3</t>
+          <t>Michigan -40.4</t>
         </is>
       </c>
       <c r="H26" t="n">
-        <v>1.5</v>
+        <v>36.5</v>
       </c>
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr"/>
@@ -1526,34 +1526,34 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Hawai'i</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Colorado State</t>
+          <t>Stanford</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>3.399999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Washington -20.5</t>
+          <t>Hawai'i -1.5</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Washington -20.5</t>
+          <t>Hawai'i -1.5</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Washington -17.1</t>
+          <t>Stanford -2.3</t>
         </is>
       </c>
       <c r="H27" t="n">
-        <v>20.5</v>
+        <v>1.5</v>
       </c>
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr"/>
@@ -1567,34 +1567,34 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Penn State</t>
+          <t>Washington</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Nevada</t>
+          <t>Colorado State</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>3.299999999999997</v>
+        <v>3.399999999999999</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Penn State -45.5</t>
+          <t>Washington -20.5</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Penn State -45.5</t>
+          <t>Washington -20.5</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Penn State -42.2</t>
+          <t>Washington -17.1</t>
         </is>
       </c>
       <c r="H28" t="n">
-        <v>45.5</v>
+        <v>20.5</v>
       </c>
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr"/>
@@ -1608,34 +1608,34 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>NC State</t>
+          <t>Penn State</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>East Carolina</t>
+          <t>Nevada</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>3.1</v>
+        <v>3.299999999999997</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>NC State -12.5</t>
+          <t>Penn State -45.5</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>NC State -12.5</t>
+          <t>Penn State -45.5</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>NC State -15.6</t>
+          <t>Penn State -42.2</t>
         </is>
       </c>
       <c r="H29" t="n">
-        <v>12.5</v>
+        <v>45.5</v>
       </c>
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr"/>
@@ -1649,34 +1649,34 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Louisiana</t>
+          <t>NC State</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Rice</t>
+          <t>East Carolina</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Louisiana -14.5</t>
+          <t>NC State -12.5</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Louisiana -14.5</t>
+          <t>NC State -12.5</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Louisiana -11.5</t>
+          <t>NC State -15.6</t>
         </is>
       </c>
       <c r="H30" t="n">
-        <v>14.5</v>
+        <v>12.5</v>
       </c>
       <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr"/>
@@ -1690,34 +1690,34 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Southern Miss</t>
+          <t>Louisiana</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Mississippi State</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Mississippi State -11.5</t>
+          <t>Louisiana -14.5</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Mississippi State -11.5</t>
+          <t>Louisiana -14.5</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Mississippi State -14.4</t>
+          <t>Louisiana -11.5</t>
         </is>
       </c>
       <c r="H31" t="n">
-        <v>-11.5</v>
+        <v>14.5</v>
       </c>
       <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr"/>
@@ -1731,34 +1731,34 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>South Carolina</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Virginia Tech</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>2.699999999999999</v>
+        <v>2.9</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Minnesota -16.5</t>
+          <t>South Carolina -8.5</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Minnesota -16.5</t>
+          <t>South Carolina -8.5</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Minnesota -19.2</t>
+          <t>South Carolina -5.6</t>
         </is>
       </c>
       <c r="H32" t="n">
-        <v>16.5</v>
+        <v>8.5</v>
       </c>
       <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr"/>
@@ -1772,34 +1772,34 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Southern Miss</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Old Dominion</t>
+          <t>Mississippi State</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>2</v>
+        <v>2.9</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Indiana -23.5</t>
+          <t>Mississippi State -11.5</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Indiana -23.5</t>
+          <t>Mississippi State -11.5</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Indiana -21.5</t>
+          <t>Mississippi State -14.4</t>
         </is>
       </c>
       <c r="H33" t="n">
-        <v>23.5</v>
+        <v>-11.5</v>
       </c>
       <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr"/>
@@ -1813,34 +1813,34 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Clemson</t>
+          <t>Minnesota</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>LSU</t>
+          <t>Buffalo</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>1.7</v>
+        <v>2.699999999999999</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Clemson -3.5</t>
+          <t>Minnesota -16.5</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Clemson -3.5</t>
+          <t>Minnesota -16.5</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Clemson -1.8</t>
+          <t>Minnesota -19.2</t>
         </is>
       </c>
       <c r="H34" t="n">
-        <v>3.5</v>
+        <v>16.5</v>
       </c>
       <c r="I34" t="inlineStr"/>
       <c r="J34" t="inlineStr"/>
@@ -1854,34 +1854,34 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Purdue</t>
+          <t>Indiana</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Ball State</t>
+          <t>Old Dominion</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>1.600000000000001</v>
+        <v>2</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Purdue -16.5</t>
+          <t>Indiana -23.5</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Purdue -16.5</t>
+          <t>Indiana -23.5</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Purdue -18.1</t>
+          <t>Indiana -21.5</t>
         </is>
       </c>
       <c r="H35" t="n">
-        <v>16.5</v>
+        <v>23.5</v>
       </c>
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr"/>
@@ -1895,34 +1895,34 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Fresno State</t>
+          <t>Kansas State</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Georgia Southern</t>
+          <t>Iowa State</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Fresno State -2.5</t>
+          <t>Kansas State -3.5</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Fresno State -2.5</t>
+          <t>Kansas State -3.5</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Fresno State -4.0</t>
+          <t>Kansas State -1.5</t>
         </is>
       </c>
       <c r="H36" t="n">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="I36" t="inlineStr"/>
       <c r="J36" t="inlineStr"/>
@@ -1936,34 +1936,34 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Rutgers</t>
+          <t>Clemson</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Ohio</t>
+          <t>LSU</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>1.300000000000001</v>
+        <v>1.7</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Rutgers -11.5</t>
+          <t>Clemson -3.5</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Rutgers -11.5</t>
+          <t>Clemson -3.5</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Rutgers -10.2</t>
+          <t>Clemson -1.8</t>
         </is>
       </c>
       <c r="H37" t="n">
-        <v>11.5</v>
+        <v>3.5</v>
       </c>
       <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr"/>
@@ -1977,34 +1977,34 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Tulane</t>
+          <t>Purdue</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Northwestern</t>
+          <t>Ball State</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>1.3</v>
+        <v>1.600000000000001</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Tulane -6.5</t>
+          <t>Purdue -16.5</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Tulane -6.5</t>
+          <t>Purdue -16.5</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Tulane -7.8</t>
+          <t>Purdue -18.1</t>
         </is>
       </c>
       <c r="H38" t="n">
-        <v>6.5</v>
+        <v>16.5</v>
       </c>
       <c r="I38" t="inlineStr"/>
       <c r="J38" t="inlineStr"/>
@@ -2018,34 +2018,34 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Maryland</t>
+          <t>Fresno State</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Florida Atlantic</t>
+          <t>Georgia Southern</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1.1</v>
+        <v>1.5</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Maryland -16.5</t>
+          <t>Fresno State -2.5</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Maryland -16.5</t>
+          <t>Fresno State -2.5</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Maryland -15.4</t>
+          <t>Fresno State -4.0</t>
         </is>
       </c>
       <c r="H39" t="n">
-        <v>16.5</v>
+        <v>2.5</v>
       </c>
       <c r="I39" t="inlineStr"/>
       <c r="J39" t="inlineStr"/>
@@ -2059,34 +2059,34 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Virginia Tech</t>
+          <t>Rutgers</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>South Carolina</t>
+          <t>Ohio</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>1</v>
+        <v>1.300000000000001</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>South Carolina -8.5</t>
+          <t>Rutgers -11.5</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>South Carolina -8.5</t>
+          <t>Rutgers -11.5</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>South Carolina -7.5</t>
+          <t>Rutgers -10.2</t>
         </is>
       </c>
       <c r="H40" t="n">
-        <v>-8.5</v>
+        <v>11.5</v>
       </c>
       <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr"/>
@@ -2100,34 +2100,34 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Kentucky</t>
+          <t>Tulane</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Toledo</t>
+          <t>Northwestern</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.9000000000000004</v>
+        <v>1.3</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Kentucky -10.0</t>
+          <t>Tulane -6.5</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Kentucky -10</t>
+          <t>Tulane -6.5</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Kentucky -9.1</t>
+          <t>Tulane -7.8</t>
         </is>
       </c>
       <c r="H41" t="n">
-        <v>10</v>
+        <v>6.5</v>
       </c>
       <c r="I41" t="inlineStr"/>
       <c r="J41" t="inlineStr"/>
@@ -2141,34 +2141,34 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Ohio State</t>
+          <t>Maryland</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Florida Atlantic</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.8999999999999999</v>
+        <v>1.1</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Ohio State -3.0</t>
+          <t>Maryland -16.5</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Ohio State -3</t>
+          <t>Maryland -16.5</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Ohio State -3.9</t>
+          <t>Maryland -15.4</t>
         </is>
       </c>
       <c r="H42" t="n">
-        <v>3</v>
+        <v>16.5</v>
       </c>
       <c r="I42" t="inlineStr"/>
       <c r="J42" t="inlineStr"/>
@@ -2182,34 +2182,34 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Cincinnati</t>
+          <t>Kentucky</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Nebraska</t>
+          <t>Toledo</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.7000000000000002</v>
+        <v>0.9000000000000004</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Nebraska -6.5</t>
+          <t>Kentucky -10.0</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Nebraska -6.5</t>
+          <t>Kentucky -10</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Nebraska -5.8</t>
+          <t>Kentucky -9.1</t>
         </is>
       </c>
       <c r="H43" t="n">
-        <v>-6.5</v>
+        <v>10</v>
       </c>
       <c r="I43" t="inlineStr"/>
       <c r="J43" t="inlineStr"/>
@@ -2223,34 +2223,34 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Texas A&amp;M</t>
+          <t>Ohio State</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>UTSA</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.3000000000000007</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -21.5</t>
+          <t>Ohio State -3.0</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -21.5</t>
+          <t>Ohio State -3</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -21.2</t>
+          <t>Ohio State -3.9</t>
         </is>
       </c>
       <c r="H44" t="n">
-        <v>21.5</v>
+        <v>3</v>
       </c>
       <c r="I44" t="inlineStr"/>
       <c r="J44" t="inlineStr"/>
@@ -2264,34 +2264,34 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Kansas</t>
+          <t>Cincinnati</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Fresno State</t>
+          <t>Nebraska</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.3000000000000007</v>
+        <v>0.7000000000000002</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Kansas -14.0</t>
+          <t>Nebraska -6.5</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Kansas -14</t>
+          <t>Nebraska -6.5</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Kansas -13.7</t>
+          <t>Nebraska -5.8</t>
         </is>
       </c>
       <c r="H45" t="n">
-        <v>14</v>
+        <v>-6.5</v>
       </c>
       <c r="I45" t="inlineStr"/>
       <c r="J45" t="inlineStr"/>
@@ -2305,34 +2305,34 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Oregon State</t>
+          <t>Texas A&amp;M</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>California</t>
+          <t>UTSA</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.2000000000000002</v>
+        <v>0.3000000000000007</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Oregon State -3.0</t>
+          <t>Texas A&amp;M -21.5</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Oregon State -3</t>
+          <t>Texas A&amp;M -21.5</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Oregon State -2.8</t>
+          <t>Texas A&amp;M -21.2</t>
         </is>
       </c>
       <c r="H46" t="n">
-        <v>3</v>
+        <v>21.5</v>
       </c>
       <c r="I46" t="inlineStr"/>
       <c r="J46" t="inlineStr"/>
@@ -2346,34 +2346,34 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Wake Forest</t>
+          <t>Kansas</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Kennesaw State</t>
+          <t>Fresno State</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0</v>
+        <v>0.3000000000000007</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Wake Forest -17.5</t>
+          <t>Kansas -14.0</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Wake Forest -17.5</t>
+          <t>Kansas -14</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Wake Forest -17.5</t>
+          <t>Kansas -13.7</t>
         </is>
       </c>
       <c r="H47" t="n">
-        <v>17.5</v>
+        <v>14</v>
       </c>
       <c r="I47" t="inlineStr"/>
       <c r="J47" t="inlineStr"/>
@@ -2387,34 +2387,34 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Iowa State</t>
+          <t>Oregon State</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Kansas State</t>
+          <t>California</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0</v>
+        <v>0.2000000000000002</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Kansas State -3.5</t>
+          <t>Oregon State -3.0</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Kansas State -3.5</t>
+          <t>Oregon State -3</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Kansas State -3.5</t>
+          <t>Oregon State -2.8</t>
         </is>
       </c>
       <c r="H48" t="n">
-        <v>-3.5</v>
+        <v>3</v>
       </c>
       <c r="I48" t="inlineStr"/>
       <c r="J48" t="inlineStr"/>
@@ -2428,1524 +2428,39 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>UNLV</t>
+          <t>USC</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Idaho State</t>
+          <t>Missouri State</t>
         </is>
       </c>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr">
         <is>
-          <t>UNLV -nan</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr"/>
+          <t>USC -34.5</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>USC -34.5</t>
+        </is>
+      </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>UNLV nan</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr"/>
+          <t>USC nan</t>
+        </is>
+      </c>
+      <c r="H49" t="n">
+        <v>34.5</v>
+      </c>
       <c r="I49" t="inlineStr"/>
       <c r="J49" t="inlineStr"/>
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr"/>
       <c r="M49" t="inlineStr"/>
     </row>
-    <row r="50">
-      <c r="A50" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>San Diego State</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>Stony Brook</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr"/>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>San Diego State -nan</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr"/>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>San Diego State nan</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr"/>
-      <c r="I50" t="inlineStr"/>
-      <c r="J50" t="inlineStr"/>
-      <c r="K50" t="inlineStr"/>
-      <c r="L50" t="inlineStr"/>
-      <c r="M50" t="inlineStr"/>
-    </row>
-    <row r="51">
-      <c r="A51" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>Bowling Green</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>Lafayette</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr"/>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>Bowling Green -nan</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr"/>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>Bowling Green nan</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr"/>
-      <c r="I51" t="inlineStr"/>
-      <c r="J51" t="inlineStr"/>
-      <c r="K51" t="inlineStr"/>
-      <c r="L51" t="inlineStr"/>
-      <c r="M51" t="inlineStr"/>
-    </row>
-    <row r="52">
-      <c r="A52" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>UL Monroe</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>St. Francis (PA)</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr"/>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>UL Monroe -nan</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr"/>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>UL Monroe nan</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr"/>
-      <c r="I52" t="inlineStr"/>
-      <c r="J52" t="inlineStr"/>
-      <c r="K52" t="inlineStr"/>
-      <c r="L52" t="inlineStr"/>
-      <c r="M52" t="inlineStr"/>
-    </row>
-    <row r="53">
-      <c r="A53" s="1" t="n">
-        <v>51</v>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>Delaware</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>Delaware State</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr"/>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>Delaware -nan</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr"/>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>Delaware nan</t>
-        </is>
-      </c>
-      <c r="H53" t="inlineStr"/>
-      <c r="I53" t="inlineStr"/>
-      <c r="J53" t="inlineStr"/>
-      <c r="K53" t="inlineStr"/>
-      <c r="L53" t="inlineStr"/>
-      <c r="M53" t="inlineStr"/>
-    </row>
-    <row r="54">
-      <c r="A54" s="1" t="n">
-        <v>52</v>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>Missouri</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>Central Arkansas</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr"/>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>Missouri -nan</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr"/>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>Missouri nan</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr"/>
-      <c r="I54" t="inlineStr"/>
-      <c r="J54" t="inlineStr"/>
-      <c r="K54" t="inlineStr"/>
-      <c r="L54" t="inlineStr"/>
-      <c r="M54" t="inlineStr"/>
-    </row>
-    <row r="55">
-      <c r="A55" s="1" t="n">
-        <v>53</v>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>Duke</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>Elon</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr"/>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>Duke -nan</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr"/>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>Duke nan</t>
-        </is>
-      </c>
-      <c r="H55" t="inlineStr"/>
-      <c r="I55" t="inlineStr"/>
-      <c r="J55" t="inlineStr"/>
-      <c r="K55" t="inlineStr"/>
-      <c r="L55" t="inlineStr"/>
-      <c r="M55" t="inlineStr"/>
-    </row>
-    <row r="56">
-      <c r="A56" s="1" t="n">
-        <v>54</v>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>Oklahoma State</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>UT Martin</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr"/>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>Oklahoma State -nan</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr"/>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>Oklahoma State nan</t>
-        </is>
-      </c>
-      <c r="H56" t="inlineStr"/>
-      <c r="I56" t="inlineStr"/>
-      <c r="J56" t="inlineStr"/>
-      <c r="K56" t="inlineStr"/>
-      <c r="L56" t="inlineStr"/>
-      <c r="M56" t="inlineStr"/>
-    </row>
-    <row r="57">
-      <c r="A57" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>Houston</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>Stephen F. Austin</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr"/>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>Houston -nan</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr"/>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>Houston nan</t>
-        </is>
-      </c>
-      <c r="H57" t="inlineStr"/>
-      <c r="I57" t="inlineStr"/>
-      <c r="J57" t="inlineStr"/>
-      <c r="K57" t="inlineStr"/>
-      <c r="L57" t="inlineStr"/>
-      <c r="M57" t="inlineStr"/>
-    </row>
-    <row r="58">
-      <c r="A58" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>UAB</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>Alabama State</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr"/>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>UAB -nan</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr"/>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>UAB nan</t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr"/>
-      <c r="I58" t="inlineStr"/>
-      <c r="J58" t="inlineStr"/>
-      <c r="K58" t="inlineStr"/>
-      <c r="L58" t="inlineStr"/>
-      <c r="M58" t="inlineStr"/>
-    </row>
-    <row r="59">
-      <c r="A59" s="1" t="n">
-        <v>57</v>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>Army</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>Tarleton State</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr"/>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>Army -nan</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr"/>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>Army nan</t>
-        </is>
-      </c>
-      <c r="H59" t="inlineStr"/>
-      <c r="I59" t="inlineStr"/>
-      <c r="J59" t="inlineStr"/>
-      <c r="K59" t="inlineStr"/>
-      <c r="L59" t="inlineStr"/>
-      <c r="M59" t="inlineStr"/>
-    </row>
-    <row r="60">
-      <c r="A60" s="1" t="n">
-        <v>58</v>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>Florida International</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>Bethune-Cookman</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr"/>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>Florida International -nan</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr"/>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>Florida International nan</t>
-        </is>
-      </c>
-      <c r="H60" t="inlineStr"/>
-      <c r="I60" t="inlineStr"/>
-      <c r="J60" t="inlineStr"/>
-      <c r="K60" t="inlineStr"/>
-      <c r="L60" t="inlineStr"/>
-      <c r="M60" t="inlineStr"/>
-    </row>
-    <row r="61">
-      <c r="A61" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>Illinois</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>Western Illinois</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr"/>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>Illinois -nan</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr"/>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>Illinois nan</t>
-        </is>
-      </c>
-      <c r="H61" t="inlineStr"/>
-      <c r="I61" t="inlineStr"/>
-      <c r="J61" t="inlineStr"/>
-      <c r="K61" t="inlineStr"/>
-      <c r="L61" t="inlineStr"/>
-      <c r="M61" t="inlineStr"/>
-    </row>
-    <row r="62">
-      <c r="A62" s="1" t="n">
-        <v>61</v>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>Navy</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>VMI</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr"/>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>Navy -nan</t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr"/>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>Navy nan</t>
-        </is>
-      </c>
-      <c r="H62" t="inlineStr"/>
-      <c r="I62" t="inlineStr"/>
-      <c r="J62" t="inlineStr"/>
-      <c r="K62" t="inlineStr"/>
-      <c r="L62" t="inlineStr"/>
-      <c r="M62" t="inlineStr"/>
-    </row>
-    <row r="63">
-      <c r="A63" s="1" t="n">
-        <v>62</v>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>Pittsburgh</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>Duquesne</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr"/>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>Pittsburgh -nan</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr"/>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>Pittsburgh nan</t>
-        </is>
-      </c>
-      <c r="H63" t="inlineStr"/>
-      <c r="I63" t="inlineStr"/>
-      <c r="J63" t="inlineStr"/>
-      <c r="K63" t="inlineStr"/>
-      <c r="L63" t="inlineStr"/>
-      <c r="M63" t="inlineStr"/>
-    </row>
-    <row r="64">
-      <c r="A64" s="1" t="n">
-        <v>63</v>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>Kent State</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>Merrimack</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr"/>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>Kent State -nan</t>
-        </is>
-      </c>
-      <c r="F64" t="inlineStr"/>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>Kent State nan</t>
-        </is>
-      </c>
-      <c r="H64" t="inlineStr"/>
-      <c r="I64" t="inlineStr"/>
-      <c r="J64" t="inlineStr"/>
-      <c r="K64" t="inlineStr"/>
-      <c r="L64" t="inlineStr"/>
-      <c r="M64" t="inlineStr"/>
-    </row>
-    <row r="65">
-      <c r="A65" s="1" t="n">
-        <v>64</v>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>UConn</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>Central Connecticut</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr"/>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>UConn -nan</t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr"/>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>UConn nan</t>
-        </is>
-      </c>
-      <c r="H65" t="inlineStr"/>
-      <c r="I65" t="inlineStr"/>
-      <c r="J65" t="inlineStr"/>
-      <c r="K65" t="inlineStr"/>
-      <c r="L65" t="inlineStr"/>
-      <c r="M65" t="inlineStr"/>
-    </row>
-    <row r="66">
-      <c r="A66" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>Boston College</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>Fordham</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr"/>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>Boston College -nan</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr"/>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>Boston College nan</t>
-        </is>
-      </c>
-      <c r="H66" t="inlineStr"/>
-      <c r="I66" t="inlineStr"/>
-      <c r="J66" t="inlineStr"/>
-      <c r="K66" t="inlineStr"/>
-      <c r="L66" t="inlineStr"/>
-      <c r="M66" t="inlineStr"/>
-    </row>
-    <row r="67">
-      <c r="A67" s="1" t="n">
-        <v>66</v>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>West Virginia</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>Robert Morris</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr"/>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>West Virginia -nan</t>
-        </is>
-      </c>
-      <c r="F67" t="inlineStr"/>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>West Virginia nan</t>
-        </is>
-      </c>
-      <c r="H67" t="inlineStr"/>
-      <c r="I67" t="inlineStr"/>
-      <c r="J67" t="inlineStr"/>
-      <c r="K67" t="inlineStr"/>
-      <c r="L67" t="inlineStr"/>
-      <c r="M67" t="inlineStr"/>
-    </row>
-    <row r="68">
-      <c r="A68" s="1" t="n">
-        <v>67</v>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>Louisville</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>Eastern Kentucky</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr"/>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>Louisville -nan</t>
-        </is>
-      </c>
-      <c r="F68" t="inlineStr"/>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>Louisville nan</t>
-        </is>
-      </c>
-      <c r="H68" t="inlineStr"/>
-      <c r="I68" t="inlineStr"/>
-      <c r="J68" t="inlineStr"/>
-      <c r="K68" t="inlineStr"/>
-      <c r="L68" t="inlineStr"/>
-      <c r="M68" t="inlineStr"/>
-    </row>
-    <row r="69">
-      <c r="A69" s="1" t="n">
-        <v>68</v>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>Air Force</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>Bucknell</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr"/>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>Air Force -nan</t>
-        </is>
-      </c>
-      <c r="F69" t="inlineStr"/>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>Air Force nan</t>
-        </is>
-      </c>
-      <c r="H69" t="inlineStr"/>
-      <c r="I69" t="inlineStr"/>
-      <c r="J69" t="inlineStr"/>
-      <c r="K69" t="inlineStr"/>
-      <c r="L69" t="inlineStr"/>
-      <c r="M69" t="inlineStr"/>
-    </row>
-    <row r="70">
-      <c r="A70" s="1" t="n">
-        <v>69</v>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>Northern Illinois</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>Holy Cross</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr"/>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>Northern Illinois -nan</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr"/>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>Northern Illinois nan</t>
-        </is>
-      </c>
-      <c r="H70" t="inlineStr"/>
-      <c r="I70" t="inlineStr"/>
-      <c r="J70" t="inlineStr"/>
-      <c r="K70" t="inlineStr"/>
-      <c r="L70" t="inlineStr"/>
-      <c r="M70" t="inlineStr"/>
-    </row>
-    <row r="71">
-      <c r="A71" s="1" t="n">
-        <v>71</v>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>Liberty</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>Maine</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr"/>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>Liberty -nan</t>
-        </is>
-      </c>
-      <c r="F71" t="inlineStr"/>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>Liberty nan</t>
-        </is>
-      </c>
-      <c r="H71" t="inlineStr"/>
-      <c r="I71" t="inlineStr"/>
-      <c r="J71" t="inlineStr"/>
-      <c r="K71" t="inlineStr"/>
-      <c r="L71" t="inlineStr"/>
-      <c r="M71" t="inlineStr"/>
-    </row>
-    <row r="72">
-      <c r="A72" s="1" t="n">
-        <v>72</v>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>Oregon</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>Montana State</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr"/>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>Oregon -nan</t>
-        </is>
-      </c>
-      <c r="F72" t="inlineStr"/>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>Oregon nan</t>
-        </is>
-      </c>
-      <c r="H72" t="inlineStr"/>
-      <c r="I72" t="inlineStr"/>
-      <c r="J72" t="inlineStr"/>
-      <c r="K72" t="inlineStr"/>
-      <c r="L72" t="inlineStr"/>
-      <c r="M72" t="inlineStr"/>
-    </row>
-    <row r="73">
-      <c r="A73" s="1" t="n">
-        <v>73</v>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>Arkansas</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>Alabama A&amp;M</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr"/>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>Arkansas -nan</t>
-        </is>
-      </c>
-      <c r="F73" t="inlineStr"/>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>Arkansas nan</t>
-        </is>
-      </c>
-      <c r="H73" t="inlineStr"/>
-      <c r="I73" t="inlineStr"/>
-      <c r="J73" t="inlineStr"/>
-      <c r="K73" t="inlineStr"/>
-      <c r="L73" t="inlineStr"/>
-      <c r="M73" t="inlineStr"/>
-    </row>
-    <row r="74">
-      <c r="A74" s="1" t="n">
-        <v>74</v>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>Memphis</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>Chattanooga</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr"/>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>Memphis -nan</t>
-        </is>
-      </c>
-      <c r="F74" t="inlineStr"/>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>Memphis nan</t>
-        </is>
-      </c>
-      <c r="H74" t="inlineStr"/>
-      <c r="I74" t="inlineStr"/>
-      <c r="J74" t="inlineStr"/>
-      <c r="K74" t="inlineStr"/>
-      <c r="L74" t="inlineStr"/>
-      <c r="M74" t="inlineStr"/>
-    </row>
-    <row r="75">
-      <c r="A75" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>James Madison</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>Weber State</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr"/>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>James Madison -nan</t>
-        </is>
-      </c>
-      <c r="F75" t="inlineStr"/>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>James Madison nan</t>
-        </is>
-      </c>
-      <c r="H75" t="inlineStr"/>
-      <c r="I75" t="inlineStr"/>
-      <c r="J75" t="inlineStr"/>
-      <c r="K75" t="inlineStr"/>
-      <c r="L75" t="inlineStr"/>
-      <c r="M75" t="inlineStr"/>
-    </row>
-    <row r="76">
-      <c r="A76" s="1" t="n">
-        <v>76</v>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>Oklahoma</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>Illinois State</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr"/>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>Oklahoma -nan</t>
-        </is>
-      </c>
-      <c r="F76" t="inlineStr"/>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>Oklahoma nan</t>
-        </is>
-      </c>
-      <c r="H76" t="inlineStr"/>
-      <c r="I76" t="inlineStr"/>
-      <c r="J76" t="inlineStr"/>
-      <c r="K76" t="inlineStr"/>
-      <c r="L76" t="inlineStr"/>
-      <c r="M76" t="inlineStr"/>
-    </row>
-    <row r="77">
-      <c r="A77" s="1" t="n">
-        <v>77</v>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>Iowa</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>UAlbany</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr"/>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>Iowa -nan</t>
-        </is>
-      </c>
-      <c r="F77" t="inlineStr"/>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>Iowa nan</t>
-        </is>
-      </c>
-      <c r="H77" t="inlineStr"/>
-      <c r="I77" t="inlineStr"/>
-      <c r="J77" t="inlineStr"/>
-      <c r="K77" t="inlineStr"/>
-      <c r="L77" t="inlineStr"/>
-      <c r="M77" t="inlineStr"/>
-    </row>
-    <row r="78">
-      <c r="A78" s="1" t="n">
-        <v>78</v>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>Vanderbilt</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>Charleston Southern</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr"/>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>Vanderbilt -nan</t>
-        </is>
-      </c>
-      <c r="F78" t="inlineStr"/>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>Vanderbilt nan</t>
-        </is>
-      </c>
-      <c r="H78" t="inlineStr"/>
-      <c r="I78" t="inlineStr"/>
-      <c r="J78" t="inlineStr"/>
-      <c r="K78" t="inlineStr"/>
-      <c r="L78" t="inlineStr"/>
-      <c r="M78" t="inlineStr"/>
-    </row>
-    <row r="79">
-      <c r="A79" s="1" t="n">
-        <v>79</v>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>Kansas State</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>North Dakota</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr"/>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>Kansas State -nan</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr"/>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>Kansas State nan</t>
-        </is>
-      </c>
-      <c r="H79" t="inlineStr"/>
-      <c r="I79" t="inlineStr"/>
-      <c r="J79" t="inlineStr"/>
-      <c r="K79" t="inlineStr"/>
-      <c r="L79" t="inlineStr"/>
-      <c r="M79" t="inlineStr"/>
-    </row>
-    <row r="80">
-      <c r="A80" s="1" t="n">
-        <v>80</v>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>Florida</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>Long Island University</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr"/>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>Florida -nan</t>
-        </is>
-      </c>
-      <c r="F80" t="inlineStr"/>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>Florida nan</t>
-        </is>
-      </c>
-      <c r="H80" t="inlineStr"/>
-      <c r="I80" t="inlineStr"/>
-      <c r="J80" t="inlineStr"/>
-      <c r="K80" t="inlineStr"/>
-      <c r="L80" t="inlineStr"/>
-      <c r="M80" t="inlineStr"/>
-    </row>
-    <row r="81">
-      <c r="A81" s="1" t="n">
-        <v>81</v>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>Troy</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>Nicholls</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr"/>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>Troy -nan</t>
-        </is>
-      </c>
-      <c r="F81" t="inlineStr"/>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>Troy nan</t>
-        </is>
-      </c>
-      <c r="H81" t="inlineStr"/>
-      <c r="I81" t="inlineStr"/>
-      <c r="J81" t="inlineStr"/>
-      <c r="K81" t="inlineStr"/>
-      <c r="L81" t="inlineStr"/>
-      <c r="M81" t="inlineStr"/>
-    </row>
-    <row r="82">
-      <c r="A82" s="1" t="n">
-        <v>82</v>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>South Alabama</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>Morgan State</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr"/>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>South Alabama -nan</t>
-        </is>
-      </c>
-      <c r="F82" t="inlineStr"/>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>South Alabama nan</t>
-        </is>
-      </c>
-      <c r="H82" t="inlineStr"/>
-      <c r="I82" t="inlineStr"/>
-      <c r="J82" t="inlineStr"/>
-      <c r="K82" t="inlineStr"/>
-      <c r="L82" t="inlineStr"/>
-      <c r="M82" t="inlineStr"/>
-    </row>
-    <row r="83">
-      <c r="A83" s="1" t="n">
-        <v>83</v>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>Arkansas State</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>Southeast Missouri State</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr"/>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>Arkansas State -nan</t>
-        </is>
-      </c>
-      <c r="F83" t="inlineStr"/>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>Arkansas State nan</t>
-        </is>
-      </c>
-      <c r="H83" t="inlineStr"/>
-      <c r="I83" t="inlineStr"/>
-      <c r="J83" t="inlineStr"/>
-      <c r="K83" t="inlineStr"/>
-      <c r="L83" t="inlineStr"/>
-      <c r="M83" t="inlineStr"/>
-    </row>
-    <row r="84">
-      <c r="A84" s="1" t="n">
-        <v>85</v>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>Middle Tennessee</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>Austin Peay</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr"/>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>Middle Tennessee -nan</t>
-        </is>
-      </c>
-      <c r="F84" t="inlineStr"/>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>Middle Tennessee nan</t>
-        </is>
-      </c>
-      <c r="H84" t="inlineStr"/>
-      <c r="I84" t="inlineStr"/>
-      <c r="J84" t="inlineStr"/>
-      <c r="K84" t="inlineStr"/>
-      <c r="L84" t="inlineStr"/>
-      <c r="M84" t="inlineStr"/>
-    </row>
-    <row r="85">
-      <c r="A85" s="1" t="n">
-        <v>86</v>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>Texas Tech</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>Arkansas-Pine Bluff</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr"/>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>Texas Tech -nan</t>
-        </is>
-      </c>
-      <c r="F85" t="inlineStr"/>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>Texas Tech nan</t>
-        </is>
-      </c>
-      <c r="H85" t="inlineStr"/>
-      <c r="I85" t="inlineStr"/>
-      <c r="J85" t="inlineStr"/>
-      <c r="K85" t="inlineStr"/>
-      <c r="L85" t="inlineStr"/>
-      <c r="M85" t="inlineStr"/>
-    </row>
-    <row r="86">
-      <c r="A86" s="1" t="n">
-        <v>87</v>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>USC</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>Missouri State</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr"/>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>USC -34.5</t>
-        </is>
-      </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>USC -34.5</t>
-        </is>
-      </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>USC nan</t>
-        </is>
-      </c>
-      <c r="H86" t="n">
-        <v>34.5</v>
-      </c>
-      <c r="I86" t="inlineStr"/>
-      <c r="J86" t="inlineStr"/>
-      <c r="K86" t="inlineStr"/>
-      <c r="L86" t="inlineStr"/>
-      <c r="M86" t="inlineStr"/>
-    </row>
-    <row r="87">
-      <c r="A87" s="1" t="n">
-        <v>88</v>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>Louisiana Tech</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>SE Louisiana</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr"/>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>Louisiana Tech -nan</t>
-        </is>
-      </c>
-      <c r="F87" t="inlineStr"/>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>Louisiana Tech nan</t>
-        </is>
-      </c>
-      <c r="H87" t="inlineStr"/>
-      <c r="I87" t="inlineStr"/>
-      <c r="J87" t="inlineStr"/>
-      <c r="K87" t="inlineStr"/>
-      <c r="L87" t="inlineStr"/>
-      <c r="M87" t="inlineStr"/>
-    </row>
-    <row r="88">
-      <c r="A88" s="1" t="n">
-        <v>89</v>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>North Texas</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>Lamar</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr"/>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t>North Texas -nan</t>
-        </is>
-      </c>
-      <c r="F88" t="inlineStr"/>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>North Texas nan</t>
-        </is>
-      </c>
-      <c r="H88" t="inlineStr"/>
-      <c r="I88" t="inlineStr"/>
-      <c r="J88" t="inlineStr"/>
-      <c r="K88" t="inlineStr"/>
-      <c r="L88" t="inlineStr"/>
-      <c r="M88" t="inlineStr"/>
-    </row>
-    <row r="89">
-      <c r="A89" s="1" t="n">
-        <v>90</v>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>BYU</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>Portland State</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr"/>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>BYU -nan</t>
-        </is>
-      </c>
-      <c r="F89" t="inlineStr"/>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>BYU nan</t>
-        </is>
-      </c>
-      <c r="H89" t="inlineStr"/>
-      <c r="I89" t="inlineStr"/>
-      <c r="J89" t="inlineStr"/>
-      <c r="K89" t="inlineStr"/>
-      <c r="L89" t="inlineStr"/>
-      <c r="M89" t="inlineStr"/>
-    </row>
-    <row r="90">
-      <c r="A90" s="1" t="n">
-        <v>91</v>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>Tulsa</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>Abilene Christian</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr"/>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>Tulsa -nan</t>
-        </is>
-      </c>
-      <c r="F90" t="inlineStr"/>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>Tulsa nan</t>
-        </is>
-      </c>
-      <c r="H90" t="inlineStr"/>
-      <c r="I90" t="inlineStr"/>
-      <c r="J90" t="inlineStr"/>
-      <c r="K90" t="inlineStr"/>
-      <c r="L90" t="inlineStr"/>
-      <c r="M90" t="inlineStr"/>
-    </row>
-    <row r="91">
-      <c r="A91" s="1" t="n">
-        <v>92</v>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>New Mexico State</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>Bryant</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr"/>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>New Mexico State -nan</t>
-        </is>
-      </c>
-      <c r="F91" t="inlineStr"/>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>New Mexico State nan</t>
-        </is>
-      </c>
-      <c r="H91" t="inlineStr"/>
-      <c r="I91" t="inlineStr"/>
-      <c r="J91" t="inlineStr"/>
-      <c r="K91" t="inlineStr"/>
-      <c r="L91" t="inlineStr"/>
-      <c r="M91" t="inlineStr"/>
-    </row>
-    <row r="92">
-      <c r="A92" s="1" t="n">
-        <v>93</v>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>SMU</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>East Texas A&amp;M</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr"/>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>SMU -nan</t>
-        </is>
-      </c>
-      <c r="F92" t="inlineStr"/>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>SMU nan</t>
-        </is>
-      </c>
-      <c r="H92" t="inlineStr"/>
-      <c r="I92" t="inlineStr"/>
-      <c r="J92" t="inlineStr"/>
-      <c r="K92" t="inlineStr"/>
-      <c r="L92" t="inlineStr"/>
-      <c r="M92" t="inlineStr"/>
-    </row>
-    <row r="93">
-      <c r="A93" s="1" t="n">
-        <v>94</v>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>Arizona State</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>Northern Arizona</t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr"/>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>Arizona State -nan</t>
-        </is>
-      </c>
-      <c r="F93" t="inlineStr"/>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>Arizona State nan</t>
-        </is>
-      </c>
-      <c r="H93" t="inlineStr"/>
-      <c r="I93" t="inlineStr"/>
-      <c r="J93" t="inlineStr"/>
-      <c r="K93" t="inlineStr"/>
-      <c r="L93" t="inlineStr"/>
-      <c r="M93" t="inlineStr"/>
-    </row>
-    <row r="94">
-      <c r="A94" s="1" t="n">
-        <v>95</v>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>Washington State</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>Idaho</t>
-        </is>
-      </c>
-      <c r="D94" t="inlineStr"/>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t>Washington State -nan</t>
-        </is>
-      </c>
-      <c r="F94" t="inlineStr"/>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>Washington State nan</t>
-        </is>
-      </c>
-      <c r="H94" t="inlineStr"/>
-      <c r="I94" t="inlineStr"/>
-      <c r="J94" t="inlineStr"/>
-      <c r="K94" t="inlineStr"/>
-      <c r="L94" t="inlineStr"/>
-      <c r="M94" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
updating HFA and ELO adjustments
</commit_message>
<xml_diff>
--- a/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week1.xlsx
+++ b/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week1.xlsx
@@ -501,34 +501,34 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ole Miss</t>
+          <t>Sam Houston</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Georgia State</t>
+          <t>UNLV</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>10</v>
+        <v>14.2</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Ole Miss -38.5</t>
+          <t>UNLV -13.5</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Ole Miss -38.5</t>
+          <t>UNLV -13.5</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Ole Miss -28.5</t>
+          <t>Sam Houston -0.7</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>38.5</v>
+        <v>-13.5</v>
       </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
@@ -542,34 +542,34 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>Virginia</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Marshall</t>
+          <t>Coastal Carolina</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>10</v>
+        <v>13.1</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Georgia -39.5</t>
+          <t>Virginia -12.5</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Georgia -39.5</t>
+          <t>Virginia -12.5</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Georgia -29.5</t>
+          <t>Coastal Carolina -0.6</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>39.5</v>
+        <v>12.5</v>
       </c>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
@@ -583,34 +583,34 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Virginia</t>
+          <t>Ole Miss</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Coastal Carolina</t>
+          <t>Georgia State</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>10</v>
+        <v>11.8</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Virginia -12.5</t>
+          <t>Ole Miss -38.5</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Virginia -12.5</t>
+          <t>Ole Miss -38.5</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Virginia -2.5</t>
+          <t>Ole Miss -26.7</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>12.5</v>
+        <v>38.5</v>
       </c>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
@@ -624,34 +624,34 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Sam Houston</t>
+          <t>South Florida</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>UNLV</t>
+          <t>Boise State</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>UNLV -13.5</t>
+          <t>Boise State -8.5</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>UNLV -13.5</t>
+          <t>Boise State -8.5</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>UNLV -3.5</t>
+          <t>South Florida -2.0</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>-13.5</v>
+        <v>-8.5</v>
       </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
@@ -665,34 +665,34 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>UCLA</t>
+          <t>Michigan State</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>Western Michigan</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>9.1</v>
+        <v>10.1</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Utah -6.5</t>
+          <t>Michigan State -18.5</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Utah -6.5</t>
+          <t>Michigan State -18.5</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>UCLA -2.6</t>
+          <t>Michigan State -8.4</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>-6.5</v>
+        <v>18.5</v>
       </c>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
@@ -706,34 +706,34 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Michigan State</t>
+          <t>UCLA</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Western Michigan</t>
+          <t>Utah</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>8.9</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Michigan State -18.5</t>
+          <t>Utah -6.5</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Michigan State -18.5</t>
+          <t>Utah -6.5</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Michigan State -9.6</t>
+          <t>UCLA -3.3</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>18.5</v>
+        <v>-6.5</v>
       </c>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
@@ -747,34 +747,34 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Texas State</t>
+          <t>Wisconsin</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Eastern Michigan</t>
+          <t>Miami (OH)</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>8.399999999999999</v>
+        <v>7.4</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Texas State -14.0</t>
+          <t>Wisconsin -17.5</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Texas State -14</t>
+          <t>Wisconsin -17.5</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Texas State -22.4</t>
+          <t>Wisconsin -10.1</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>14</v>
+        <v>17.5</v>
       </c>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
@@ -788,34 +788,34 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Arizona</t>
+          <t>Penn State</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Hawai'i</t>
+          <t>Nevada</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>8.399999999999999</v>
+        <v>7.299999999999997</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Arizona -13.5</t>
+          <t>Penn State -45.5</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Arizona -13.5</t>
+          <t>Penn State -45.5</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Arizona -21.9</t>
+          <t>Penn State -38.2</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>13.5</v>
+        <v>45.5</v>
       </c>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
@@ -829,34 +829,34 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Western Kentucky</t>
+          <t>Baylor</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Sam Houston</t>
+          <t>Auburn</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>7.9</v>
+        <v>6.5</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Western Kentucky -9.5</t>
+          <t>Auburn -1.5</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Western Kentucky -9.5</t>
+          <t>Auburn -1.5</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Western Kentucky -1.6</t>
+          <t>Baylor -5.0</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>9.5</v>
+        <v>-1.5</v>
       </c>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
@@ -870,34 +870,34 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>San José State</t>
+          <t>Washington</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Central Michigan</t>
+          <t>Colorado State</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>7.899999999999999</v>
+        <v>6.1</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>San José State -11.5</t>
+          <t>Washington -20.5</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>San José State -11.5</t>
+          <t>Washington -20.5</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>San José State -19.4</t>
+          <t>Washington -14.4</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>11.5</v>
+        <v>20.5</v>
       </c>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
@@ -911,34 +911,34 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>South Florida</t>
+          <t>Arizona</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Boise State</t>
+          <t>Hawai'i</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>7.8</v>
+        <v>6</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Boise State -8.5</t>
+          <t>Arizona -13.5</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Boise State -8.5</t>
+          <t>Arizona -13.5</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Boise State -0.7</t>
+          <t>Arizona -19.5</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>-8.5</v>
+        <v>13.5</v>
       </c>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
@@ -952,34 +952,34 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Utah State</t>
+          <t>Akron</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>UTEP</t>
+          <t>Wyoming</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>7.699999999999999</v>
+        <v>5.9</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Utah State -3.5</t>
+          <t>Wyoming -8.5</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Utah State -3.5</t>
+          <t>Wyoming -8.5</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Utah State -11.2</t>
+          <t>Wyoming -2.6</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>3.5</v>
+        <v>-8.5</v>
       </c>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
@@ -993,34 +993,34 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Wisconsin</t>
+          <t>Western Kentucky</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Miami (OH)</t>
+          <t>Sam Houston</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>7.4</v>
+        <v>5.6</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Wisconsin -17.5</t>
+          <t>Western Kentucky -9.5</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Wisconsin -17.5</t>
+          <t>Western Kentucky -9.5</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Wisconsin -10.1</t>
+          <t>Western Kentucky -3.9</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>17.5</v>
+        <v>9.5</v>
       </c>
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
@@ -1034,34 +1034,34 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Florida State</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Alabama</t>
+          <t>Marshall</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>7.399999999999999</v>
+        <v>5.5</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Alabama -13.5</t>
+          <t>Georgia -39.5</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Alabama -13.5</t>
+          <t>Georgia -39.5</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Alabama -20.9</t>
+          <t>Georgia -34.0</t>
         </is>
       </c>
       <c r="H15" t="n">
-        <v>-13.5</v>
+        <v>39.5</v>
       </c>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
@@ -1075,34 +1075,34 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Baylor</t>
+          <t>Louisiana</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Auburn</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>6.5</v>
+        <v>5.4</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Auburn -1.5</t>
+          <t>Louisiana -14.5</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Auburn -1.5</t>
+          <t>Louisiana -14.5</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Baylor -5.0</t>
+          <t>Louisiana -9.1</t>
         </is>
       </c>
       <c r="H16" t="n">
-        <v>-1.5</v>
+        <v>14.5</v>
       </c>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
@@ -1116,34 +1116,34 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>UCF</t>
+          <t>Indiana</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Jacksonville State</t>
+          <t>Old Dominion</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>5.6</v>
+        <v>5.100000000000001</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>UCF -16.5</t>
+          <t>Indiana -23.5</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>UCF -16.5</t>
+          <t>Indiana -23.5</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>UCF -10.9</t>
+          <t>Indiana -18.4</t>
         </is>
       </c>
       <c r="H17" t="n">
-        <v>16.5</v>
+        <v>23.5</v>
       </c>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
@@ -1157,34 +1157,34 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Akron</t>
+          <t>Hawai'i</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Wyoming</t>
+          <t>Stanford</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>5.4</v>
+        <v>4.9</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Wyoming -8.5</t>
+          <t>Hawai'i -1.5</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Wyoming -8.5</t>
+          <t>Hawai'i -1.5</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Wyoming -3.1</t>
+          <t>Stanford -3.4</t>
         </is>
       </c>
       <c r="H18" t="n">
-        <v>-8.5</v>
+        <v>1.5</v>
       </c>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
@@ -1198,34 +1198,34 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Colorado</t>
+          <t>Texas State</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Georgia Tech</t>
+          <t>Eastern Michigan</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>5.3</v>
+        <v>4.899999999999999</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Georgia Tech -4.0</t>
+          <t>Texas State -14.0</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Georgia Tech -4</t>
+          <t>Texas State -14</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Colorado -1.3</t>
+          <t>Texas State -18.9</t>
         </is>
       </c>
       <c r="H19" t="n">
-        <v>-4</v>
+        <v>14</v>
       </c>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
@@ -1239,34 +1239,34 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Wake Forest</t>
+          <t>Utah State</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Kennesaw State</t>
+          <t>UTEP</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>5.100000000000001</v>
+        <v>4.800000000000001</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Wake Forest -17.5</t>
+          <t>Utah State -3.5</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Wake Forest -17.5</t>
+          <t>Utah State -3.5</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Wake Forest -22.6</t>
+          <t>Utah State -8.3</t>
         </is>
       </c>
       <c r="H20" t="n">
-        <v>17.5</v>
+        <v>3.5</v>
       </c>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
@@ -1280,34 +1280,34 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>San José State</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>App State</t>
+          <t>Central Michigan</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>4.4</v>
+        <v>4.600000000000001</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>App State -8.5</t>
+          <t>San José State -11.5</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>App State -8.5</t>
+          <t>San José State -11.5</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>App State -12.9</t>
+          <t>San José State -16.1</t>
         </is>
       </c>
       <c r="H21" t="n">
-        <v>-8.5</v>
+        <v>11.5</v>
       </c>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
@@ -1321,34 +1321,34 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Notre Dame</t>
+          <t>Georgia Tech</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>4.4</v>
+        <v>4.3</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Notre Dame -2.5</t>
+          <t>Georgia Tech -4.0</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Notre Dame -2.5</t>
+          <t>Georgia Tech -4</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Notre Dame -6.9</t>
+          <t>Colorado -0.3</t>
         </is>
       </c>
       <c r="H22" t="n">
-        <v>-2.5</v>
+        <v>-4</v>
       </c>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
@@ -1362,34 +1362,34 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>North Carolina</t>
+          <t>UCF</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>TCU</t>
+          <t>Jacksonville State</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>4.2</v>
+        <v>3.699999999999999</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>TCU -3.0</t>
+          <t>UCF -16.5</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>TCU -3</t>
+          <t>UCF -16.5</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>TCU -7.2</t>
+          <t>UCF -12.8</t>
         </is>
       </c>
       <c r="H23" t="n">
-        <v>-3</v>
+        <v>16.5</v>
       </c>
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
@@ -1403,30 +1403,30 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Syracuse</t>
+          <t>Florida State</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Tennessee</t>
+          <t>Alabama</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>4.100000000000001</v>
+        <v>3.699999999999999</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Tennessee -13.5</t>
+          <t>Alabama -13.5</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Tennessee -13.5</t>
+          <t>Alabama -13.5</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Tennessee -17.6</t>
+          <t>Alabama -17.2</t>
         </is>
       </c>
       <c r="H24" t="n">
@@ -1444,34 +1444,34 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Massachusetts</t>
+          <t>South Carolina</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Temple</t>
+          <t>Virginia Tech</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>3.9</v>
+        <v>3.5</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Temple -3.0</t>
+          <t>South Carolina -8.5</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Temple -3</t>
+          <t>South Carolina -8.5</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Massachusetts -0.9</t>
+          <t>South Carolina -5.0</t>
         </is>
       </c>
       <c r="H25" t="n">
-        <v>-3</v>
+        <v>8.5</v>
       </c>
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
@@ -1485,34 +1485,34 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Michigan</t>
+          <t>Maryland</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>New Mexico</t>
+          <t>Florida Atlantic</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>3.899999999999999</v>
+        <v>3.4</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Michigan -36.5</t>
+          <t>Maryland -16.5</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Michigan -36.5</t>
+          <t>Maryland -16.5</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Michigan -40.4</t>
+          <t>Maryland -13.1</t>
         </is>
       </c>
       <c r="H26" t="n">
-        <v>36.5</v>
+        <v>16.5</v>
       </c>
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr"/>
@@ -1526,34 +1526,34 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Hawai'i</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Stanford</t>
+          <t>App State</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>3.8</v>
+        <v>2.9</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Hawai'i -1.5</t>
+          <t>App State -8.5</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Hawai'i -1.5</t>
+          <t>App State -8.5</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Stanford -2.3</t>
+          <t>App State -11.4</t>
         </is>
       </c>
       <c r="H27" t="n">
-        <v>1.5</v>
+        <v>-8.5</v>
       </c>
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr"/>
@@ -1567,34 +1567,34 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Wake Forest</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Colorado State</t>
+          <t>Kennesaw State</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>3.399999999999999</v>
+        <v>2.5</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Washington -20.5</t>
+          <t>Wake Forest -17.5</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Washington -20.5</t>
+          <t>Wake Forest -17.5</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Washington -17.1</t>
+          <t>Wake Forest -20.0</t>
         </is>
       </c>
       <c r="H28" t="n">
-        <v>20.5</v>
+        <v>17.5</v>
       </c>
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr"/>
@@ -1608,34 +1608,34 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Penn State</t>
+          <t>North Carolina</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Nevada</t>
+          <t>TCU</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>3.299999999999997</v>
+        <v>2.2</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Penn State -45.5</t>
+          <t>TCU -3.0</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Penn State -45.5</t>
+          <t>TCU -3</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Penn State -42.2</t>
+          <t>TCU -5.2</t>
         </is>
       </c>
       <c r="H29" t="n">
-        <v>45.5</v>
+        <v>-3</v>
       </c>
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr"/>
@@ -1649,34 +1649,34 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>NC State</t>
+          <t>Massachusetts</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>East Carolina</t>
+          <t>Temple</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>3.1</v>
+        <v>2.1</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>NC State -12.5</t>
+          <t>Temple -3.0</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>NC State -12.5</t>
+          <t>Temple -3</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>NC State -15.6</t>
+          <t>Temple -0.9</t>
         </is>
       </c>
       <c r="H30" t="n">
-        <v>12.5</v>
+        <v>-3</v>
       </c>
       <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr"/>
@@ -1690,34 +1690,34 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Louisiana</t>
+          <t>NC State</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Rice</t>
+          <t>East Carolina</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>3</v>
+        <v>1.9</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Louisiana -14.5</t>
+          <t>NC State -12.5</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Louisiana -14.5</t>
+          <t>NC State -12.5</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Louisiana -11.5</t>
+          <t>NC State -14.4</t>
         </is>
       </c>
       <c r="H31" t="n">
-        <v>14.5</v>
+        <v>12.5</v>
       </c>
       <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr"/>
@@ -1731,34 +1731,34 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>South Carolina</t>
+          <t>Kansas State</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Virginia Tech</t>
+          <t>Iowa State</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>2.9</v>
+        <v>1.9</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>South Carolina -8.5</t>
+          <t>Kansas State -3.5</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>South Carolina -8.5</t>
+          <t>Kansas State -3.5</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>South Carolina -5.6</t>
+          <t>Kansas State -1.6</t>
         </is>
       </c>
       <c r="H32" t="n">
-        <v>8.5</v>
+        <v>3.5</v>
       </c>
       <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr"/>
@@ -1772,34 +1772,34 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Southern Miss</t>
+          <t>Texas A&amp;M</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Mississippi State</t>
+          <t>UTSA</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>2.9</v>
+        <v>1.800000000000001</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Mississippi State -11.5</t>
+          <t>Texas A&amp;M -21.5</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Mississippi State -11.5</t>
+          <t>Texas A&amp;M -21.5</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Mississippi State -14.4</t>
+          <t>Texas A&amp;M -19.7</t>
         </is>
       </c>
       <c r="H33" t="n">
-        <v>-11.5</v>
+        <v>21.5</v>
       </c>
       <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr"/>
@@ -1813,34 +1813,34 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Kentucky</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Toledo</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>2.699999999999999</v>
+        <v>1.800000000000001</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Minnesota -16.5</t>
+          <t>Kentucky -10.0</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Minnesota -16.5</t>
+          <t>Kentucky -10</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Minnesota -19.2</t>
+          <t>Kentucky -8.2</t>
         </is>
       </c>
       <c r="H34" t="n">
-        <v>16.5</v>
+        <v>10</v>
       </c>
       <c r="I34" t="inlineStr"/>
       <c r="J34" t="inlineStr"/>
@@ -1854,34 +1854,34 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Ohio State</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Old Dominion</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>2</v>
+        <v>1.6</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Indiana -23.5</t>
+          <t>Ohio State -3.0</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Indiana -23.5</t>
+          <t>Ohio State -3</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Indiana -21.5</t>
+          <t>Ohio State -4.6</t>
         </is>
       </c>
       <c r="H35" t="n">
-        <v>23.5</v>
+        <v>3</v>
       </c>
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr"/>
@@ -1895,34 +1895,34 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Kansas State</t>
+          <t>Kansas</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Iowa State</t>
+          <t>Fresno State</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Kansas State -3.5</t>
+          <t>Kansas -14.0</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Kansas State -3.5</t>
+          <t>Kansas -14</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Kansas State -1.5</t>
+          <t>Kansas -12.5</t>
         </is>
       </c>
       <c r="H36" t="n">
-        <v>3.5</v>
+        <v>14</v>
       </c>
       <c r="I36" t="inlineStr"/>
       <c r="J36" t="inlineStr"/>
@@ -1936,34 +1936,34 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Clemson</t>
+          <t>Cincinnati</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>LSU</t>
+          <t>Nebraska</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>1.7</v>
+        <v>1.4</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Clemson -3.5</t>
+          <t>Nebraska -6.5</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Clemson -3.5</t>
+          <t>Nebraska -6.5</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Clemson -1.8</t>
+          <t>Nebraska -5.1</t>
         </is>
       </c>
       <c r="H37" t="n">
-        <v>3.5</v>
+        <v>-6.5</v>
       </c>
       <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr"/>
@@ -1977,34 +1977,34 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Purdue</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Ball State</t>
+          <t>Notre Dame</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>1.600000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Purdue -16.5</t>
+          <t>Notre Dame -2.5</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Purdue -16.5</t>
+          <t>Notre Dame -2.5</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Purdue -18.1</t>
+          <t>Notre Dame -3.6</t>
         </is>
       </c>
       <c r="H38" t="n">
-        <v>16.5</v>
+        <v>-2.5</v>
       </c>
       <c r="I38" t="inlineStr"/>
       <c r="J38" t="inlineStr"/>
@@ -2018,34 +2018,34 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Fresno State</t>
+          <t>Oregon State</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Georgia Southern</t>
+          <t>California</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1.5</v>
+        <v>1.1</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Fresno State -2.5</t>
+          <t>Oregon State -3.0</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Fresno State -2.5</t>
+          <t>Oregon State -3</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Fresno State -4.0</t>
+          <t>Oregon State -4.1</t>
         </is>
       </c>
       <c r="H39" t="n">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="I39" t="inlineStr"/>
       <c r="J39" t="inlineStr"/>
@@ -2059,34 +2059,34 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Rutgers</t>
+          <t>Tulane</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Ohio</t>
+          <t>Northwestern</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>1.300000000000001</v>
+        <v>1</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Rutgers -11.5</t>
+          <t>Tulane -6.5</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Rutgers -11.5</t>
+          <t>Tulane -6.5</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Rutgers -10.2</t>
+          <t>Tulane -5.5</t>
         </is>
       </c>
       <c r="H40" t="n">
-        <v>11.5</v>
+        <v>6.5</v>
       </c>
       <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr"/>
@@ -2100,34 +2100,34 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Tulane</t>
+          <t>Fresno State</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Northwestern</t>
+          <t>Georgia Southern</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>1.3</v>
+        <v>0.7999999999999998</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Tulane -6.5</t>
+          <t>Fresno State -2.5</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Tulane -6.5</t>
+          <t>Fresno State -2.5</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Tulane -7.8</t>
+          <t>Fresno State -3.3</t>
         </is>
       </c>
       <c r="H41" t="n">
-        <v>6.5</v>
+        <v>2.5</v>
       </c>
       <c r="I41" t="inlineStr"/>
       <c r="J41" t="inlineStr"/>
@@ -2141,34 +2141,34 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Maryland</t>
+          <t>Syracuse</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Florida Atlantic</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1.1</v>
+        <v>0.6999999999999993</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Maryland -16.5</t>
+          <t>Tennessee -13.5</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Maryland -16.5</t>
+          <t>Tennessee -13.5</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Maryland -15.4</t>
+          <t>Tennessee -14.2</t>
         </is>
       </c>
       <c r="H42" t="n">
-        <v>16.5</v>
+        <v>-13.5</v>
       </c>
       <c r="I42" t="inlineStr"/>
       <c r="J42" t="inlineStr"/>
@@ -2182,34 +2182,34 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Kentucky</t>
+          <t>Southern Miss</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Toledo</t>
+          <t>Mississippi State</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.9000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Kentucky -10.0</t>
+          <t>Mississippi State -11.5</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Kentucky -10</t>
+          <t>Mississippi State -11.5</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Kentucky -9.1</t>
+          <t>Mississippi State -12.0</t>
         </is>
       </c>
       <c r="H43" t="n">
-        <v>10</v>
+        <v>-11.5</v>
       </c>
       <c r="I43" t="inlineStr"/>
       <c r="J43" t="inlineStr"/>
@@ -2223,34 +2223,34 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Ohio State</t>
+          <t>Rutgers</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Ohio</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.8999999999999999</v>
+        <v>0.4000000000000004</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Ohio State -3.0</t>
+          <t>Rutgers -11.5</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Ohio State -3</t>
+          <t>Rutgers -11.5</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Ohio State -3.9</t>
+          <t>Rutgers -11.9</t>
         </is>
       </c>
       <c r="H44" t="n">
-        <v>3</v>
+        <v>11.5</v>
       </c>
       <c r="I44" t="inlineStr"/>
       <c r="J44" t="inlineStr"/>
@@ -2264,34 +2264,34 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Cincinnati</t>
+          <t>Clemson</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Nebraska</t>
+          <t>LSU</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.7000000000000002</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Nebraska -6.5</t>
+          <t>Clemson -3.5</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Nebraska -6.5</t>
+          <t>Clemson -3.5</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Nebraska -5.8</t>
+          <t>Clemson -3.1</t>
         </is>
       </c>
       <c r="H45" t="n">
-        <v>-6.5</v>
+        <v>3.5</v>
       </c>
       <c r="I45" t="inlineStr"/>
       <c r="J45" t="inlineStr"/>
@@ -2305,34 +2305,34 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Texas A&amp;M</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>UTSA</t>
+          <t>New Mexico</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.3000000000000007</v>
+        <v>0.2000000000000028</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -21.5</t>
+          <t>Michigan -36.5</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -21.5</t>
+          <t>Michigan -36.5</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -21.2</t>
+          <t>Michigan -36.7</t>
         </is>
       </c>
       <c r="H46" t="n">
-        <v>21.5</v>
+        <v>36.5</v>
       </c>
       <c r="I46" t="inlineStr"/>
       <c r="J46" t="inlineStr"/>
@@ -2346,34 +2346,34 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Kansas</t>
+          <t>Minnesota</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Fresno State</t>
+          <t>Buffalo</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.3000000000000007</v>
+        <v>0.1999999999999993</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Kansas -14.0</t>
+          <t>Minnesota -16.5</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Kansas -14</t>
+          <t>Minnesota -16.5</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Kansas -13.7</t>
+          <t>Minnesota -16.7</t>
         </is>
       </c>
       <c r="H47" t="n">
-        <v>14</v>
+        <v>16.5</v>
       </c>
       <c r="I47" t="inlineStr"/>
       <c r="J47" t="inlineStr"/>
@@ -2387,34 +2387,34 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Oregon State</t>
+          <t>Purdue</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>California</t>
+          <t>Ball State</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.2000000000000002</v>
+        <v>0.1000000000000014</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Oregon State -3.0</t>
+          <t>Purdue -16.5</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Oregon State -3</t>
+          <t>Purdue -16.5</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Oregon State -2.8</t>
+          <t>Purdue -16.6</t>
         </is>
       </c>
       <c r="H48" t="n">
-        <v>3</v>
+        <v>16.5</v>
       </c>
       <c r="I48" t="inlineStr"/>
       <c r="J48" t="inlineStr"/>

</xml_diff>

<commit_message>
updating spreds with the final preseason ratings
</commit_message>
<xml_diff>
--- a/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week1.xlsx
+++ b/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M49"/>
+  <dimension ref="A1:M68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -510,7 +510,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>14.5</v>
+        <v>15.2</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -524,7 +524,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Sam Houston -1.0</t>
+          <t>Sam Houston -1.7</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -542,34 +542,34 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Virginia</t>
+          <t>Ole Miss</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Coastal Carolina</t>
+          <t>Georgia State</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>13.7</v>
+        <v>14.8</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Virginia -12.5</t>
+          <t>Ole Miss -38.5</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Virginia -12.5</t>
+          <t>Ole Miss -38.5</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Coastal Carolina -1.2</t>
+          <t>Ole Miss -23.7</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>12.5</v>
+        <v>38.5</v>
       </c>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
@@ -583,34 +583,34 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Ole Miss</t>
+          <t>Virginia</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Georgia State</t>
+          <t>Coastal Carolina</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>12.6</v>
+        <v>14.7</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Ole Miss -38.5</t>
+          <t>Virginia -12.5</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Ole Miss -38.5</t>
+          <t>Virginia -12.5</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Ole Miss -25.9</t>
+          <t>Coastal Carolina -2.2</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>38.5</v>
+        <v>12.5</v>
       </c>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
@@ -624,34 +624,34 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>South Florida</t>
+          <t>Michigan State</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Boise State</t>
+          <t>Western Michigan</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>10.4</v>
+        <v>11.1</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Boise State -8.5</t>
+          <t>Michigan State -18.5</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Boise State -8.5</t>
+          <t>Michigan State -18.5</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>South Florida -1.9</t>
+          <t>Michigan State -7.4</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>-8.5</v>
+        <v>18.5</v>
       </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
@@ -665,34 +665,34 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Michigan State</t>
+          <t>South Florida</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Western Michigan</t>
+          <t>Boise State</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>10.2</v>
+        <v>9.1</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Michigan State -18.5</t>
+          <t>Boise State -8.5</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Michigan State -18.5</t>
+          <t>Boise State -8.5</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Michigan State -8.3</t>
+          <t>South Florida -0.6</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>18.5</v>
+        <v>-8.5</v>
       </c>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
@@ -706,34 +706,34 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>UCLA</t>
+          <t>Baylor</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>Auburn</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>9.4</v>
+        <v>7.7</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Utah -6.5</t>
+          <t>Auburn -1.5</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Utah -6.5</t>
+          <t>Auburn -1.5</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>UCLA -2.9</t>
+          <t>Baylor -6.2</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>-6.5</v>
+        <v>-1.5</v>
       </c>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
@@ -747,34 +747,34 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Wisconsin</t>
+          <t>Texas State</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Miami (OH)</t>
+          <t>Eastern Michigan</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>7.9</v>
+        <v>7.699999999999999</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Wisconsin -17.5</t>
+          <t>Texas State -14.0</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Wisconsin -17.5</t>
+          <t>Texas State -14</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Wisconsin -9.6</t>
+          <t>Texas State -21.7</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>17.5</v>
+        <v>14</v>
       </c>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
@@ -788,34 +788,34 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Arizona</t>
+          <t>Utah State</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Hawai'i</t>
+          <t>UTEP</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>7.199999999999999</v>
+        <v>7.699999999999999</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Arizona -13.5</t>
+          <t>Utah State -3.5</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Arizona -13.5</t>
+          <t>Utah State -3.5</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Arizona -20.7</t>
+          <t>Utah State -11.2</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>13.5</v>
+        <v>3.5</v>
       </c>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
@@ -829,34 +829,34 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Penn State</t>
+          <t>Arizona</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Nevada</t>
+          <t>Hawai'i</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>7.100000000000001</v>
+        <v>7.699999999999999</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Penn State -45.5</t>
+          <t>Arizona -13.5</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Penn State -45.5</t>
+          <t>Arizona -13.5</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Penn State -38.4</t>
+          <t>Arizona -21.2</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>45.5</v>
+        <v>13.5</v>
       </c>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
@@ -879,7 +879,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>6.600000000000001</v>
+        <v>7.5</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -893,7 +893,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Indiana -16.9</t>
+          <t>Indiana -16.0</t>
         </is>
       </c>
       <c r="H11" t="n">
@@ -911,34 +911,34 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Baylor</t>
+          <t>Wisconsin</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Auburn</t>
+          <t>Miami (OH)</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>6.4</v>
+        <v>7.1</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Auburn -1.5</t>
+          <t>Wisconsin -17.5</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Auburn -1.5</t>
+          <t>Wisconsin -17.5</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Baylor -4.9</t>
+          <t>Wisconsin -10.4</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>-1.5</v>
+        <v>17.5</v>
       </c>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
@@ -952,34 +952,34 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Western Kentucky</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Colorado State</t>
+          <t>Sam Houston</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>6</v>
+        <v>6.2</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Washington -20.5</t>
+          <t>Western Kentucky -9.5</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Washington -20.5</t>
+          <t>Western Kentucky -9.5</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Washington -14.5</t>
+          <t>Western Kentucky -3.3</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>20.5</v>
+        <v>9.5</v>
       </c>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
@@ -993,34 +993,34 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>San José State</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Marshall</t>
+          <t>Central Michigan</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>5.799999999999997</v>
+        <v>5.899999999999999</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Georgia -39.5</t>
+          <t>San José State -11.5</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Georgia -39.5</t>
+          <t>San José State -11.5</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Georgia -33.7</t>
+          <t>San José State -17.4</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>39.5</v>
+        <v>11.5</v>
       </c>
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
@@ -1034,34 +1034,34 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Louisiana</t>
+          <t>UCF</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Rice</t>
+          <t>Jacksonville State</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>5.6</v>
+        <v>5.5</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Louisiana -14.5</t>
+          <t>UCF -16.5</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Louisiana -14.5</t>
+          <t>UCF -16.5</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Louisiana -8.9</t>
+          <t>UCF -11.0</t>
         </is>
       </c>
       <c r="H15" t="n">
-        <v>14.5</v>
+        <v>16.5</v>
       </c>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
@@ -1075,34 +1075,34 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Western Kentucky</t>
+          <t>Penn State</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Sam Houston</t>
+          <t>Nevada</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>5.5</v>
+        <v>4.799999999999997</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Western Kentucky -9.5</t>
+          <t>Penn State -45.5</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Western Kentucky -9.5</t>
+          <t>Penn State -45.5</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Western Kentucky -4.0</t>
+          <t>Penn State -40.7</t>
         </is>
       </c>
       <c r="H16" t="n">
-        <v>9.5</v>
+        <v>45.5</v>
       </c>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
@@ -1116,34 +1116,34 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>San José State</t>
+          <t>Oregon State</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Central Michigan</t>
+          <t>California</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>4.899999999999999</v>
+        <v>4.2</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>San José State -11.5</t>
+          <t>Oregon State -3.0</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>San José State -11.5</t>
+          <t>Oregon State -3</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>San José State -16.4</t>
+          <t>Oregon State -7.2</t>
         </is>
       </c>
       <c r="H17" t="n">
-        <v>11.5</v>
+        <v>3</v>
       </c>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
@@ -1157,30 +1157,30 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Akron</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Wyoming</t>
+          <t>App State</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>4.8</v>
+        <v>4.1</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Wyoming -8.5</t>
+          <t>App State -8.5</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Wyoming -8.5</t>
+          <t>App State -8.5</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Wyoming -3.7</t>
+          <t>App State -12.6</t>
         </is>
       </c>
       <c r="H18" t="n">
@@ -1198,34 +1198,34 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Hawai'i</t>
+          <t>Massachusetts</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Stanford</t>
+          <t>Temple</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>4.7</v>
+        <v>4</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Hawai'i -1.5</t>
+          <t>Temple -3.0</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Hawai'i -1.5</t>
+          <t>Temple -3</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Stanford -3.2</t>
+          <t>Massachusetts -1.0</t>
         </is>
       </c>
       <c r="H19" t="n">
-        <v>1.5</v>
+        <v>-3</v>
       </c>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
@@ -1239,34 +1239,34 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Texas State</t>
+          <t>Hawai'i</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Eastern Michigan</t>
+          <t>Stanford</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>4.699999999999999</v>
+        <v>4</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Texas State -14.0</t>
+          <t>Hawai'i -1.5</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Texas State -14</t>
+          <t>Hawai'i -1.5</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Texas State -18.7</t>
+          <t>Stanford -2.5</t>
         </is>
       </c>
       <c r="H20" t="n">
-        <v>14</v>
+        <v>1.5</v>
       </c>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
@@ -1280,34 +1280,34 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Utah State</t>
+          <t>Akron</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>UTEP</t>
+          <t>Wyoming</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>4.3</v>
+        <v>3.9</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Utah State -3.5</t>
+          <t>Wyoming -8.5</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Utah State -3.5</t>
+          <t>Wyoming -8.5</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Utah State -7.8</t>
+          <t>Wyoming -4.6</t>
         </is>
       </c>
       <c r="H21" t="n">
-        <v>3.5</v>
+        <v>-8.5</v>
       </c>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
@@ -1321,34 +1321,34 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>South Carolina</t>
+          <t>Louisiana</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Virginia Tech</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>4.3</v>
+        <v>3.800000000000001</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>South Carolina -8.5</t>
+          <t>Louisiana -14.5</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>South Carolina -8.5</t>
+          <t>Louisiana -14.5</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>South Carolina -4.2</t>
+          <t>Louisiana -10.7</t>
         </is>
       </c>
       <c r="H22" t="n">
-        <v>8.5</v>
+        <v>14.5</v>
       </c>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
@@ -1362,34 +1362,34 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Colorado</t>
+          <t>Washington</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Georgia Tech</t>
+          <t>Colorado State</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>3.9</v>
+        <v>3.600000000000001</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Georgia Tech -4.0</t>
+          <t>Washington -20.5</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Georgia Tech -4</t>
+          <t>Washington -20.5</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Georgia Tech -0.1</t>
+          <t>Washington -16.9</t>
         </is>
       </c>
       <c r="H23" t="n">
-        <v>-4</v>
+        <v>20.5</v>
       </c>
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
@@ -1412,7 +1412,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Maryland -12.9</t>
+          <t>Maryland -13.0</t>
         </is>
       </c>
       <c r="H24" t="n">
@@ -1444,12 +1444,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>UCF</t>
+          <t>Texas A&amp;M</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Jacksonville State</t>
+          <t>UTSA</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1457,21 +1457,21 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>UCF -16.5</t>
+          <t>Texas A&amp;M -21.5</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>UCF -16.5</t>
+          <t>Texas A&amp;M -21.5</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>UCF -13.0</t>
+          <t>Texas A&amp;M -25.0</t>
         </is>
       </c>
       <c r="H25" t="n">
-        <v>16.5</v>
+        <v>21.5</v>
       </c>
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
@@ -1485,34 +1485,34 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>App State</t>
+          <t>Marshall</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>3.4</v>
+        <v>3.399999999999999</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>App State -8.5</t>
+          <t>Georgia -39.5</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>App State -8.5</t>
+          <t>Georgia -39.5</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>App State -11.9</t>
+          <t>Georgia -36.1</t>
         </is>
       </c>
       <c r="H26" t="n">
-        <v>-8.5</v>
+        <v>39.5</v>
       </c>
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr"/>
@@ -1526,34 +1526,34 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Kentucky</t>
+          <t>Florida State</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Toledo</t>
+          <t>Alabama</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>2.7</v>
+        <v>3.100000000000001</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Kentucky -10.0</t>
+          <t>Alabama -13.5</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Kentucky -10</t>
+          <t>Alabama -13.5</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Kentucky -7.3</t>
+          <t>Alabama -16.6</t>
         </is>
       </c>
       <c r="H27" t="n">
-        <v>10</v>
+        <v>-13.5</v>
       </c>
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr"/>
@@ -1567,34 +1567,34 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Wake Forest</t>
+          <t>UCLA</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Kennesaw State</t>
+          <t>Utah</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>2.600000000000001</v>
+        <v>3</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Wake Forest -17.5</t>
+          <t>Utah -6.5</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Wake Forest -17.5</t>
+          <t>Utah -6.5</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Wake Forest -20.1</t>
+          <t>Utah -3.5</t>
         </is>
       </c>
       <c r="H28" t="n">
-        <v>17.5</v>
+        <v>-6.5</v>
       </c>
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr"/>
@@ -1608,34 +1608,34 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Massachusetts</t>
+          <t>South Carolina</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Temple</t>
+          <t>Virginia Tech</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>2.4</v>
+        <v>2.8</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Temple -3.0</t>
+          <t>South Carolina -8.5</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Temple -3</t>
+          <t>South Carolina -8.5</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Temple -0.6</t>
+          <t>South Carolina -5.7</t>
         </is>
       </c>
       <c r="H29" t="n">
-        <v>-3</v>
+        <v>8.5</v>
       </c>
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr"/>
@@ -1649,34 +1649,34 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>NC State</t>
+          <t>Cincinnati</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>East Carolina</t>
+          <t>Nebraska</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>2.300000000000001</v>
+        <v>2.7</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>NC State -12.5</t>
+          <t>Nebraska -6.5</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>NC State -12.5</t>
+          <t>Nebraska -6.5</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>NC State -14.8</t>
+          <t>Nebraska -3.8</t>
         </is>
       </c>
       <c r="H30" t="n">
-        <v>12.5</v>
+        <v>-6.5</v>
       </c>
       <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr"/>
@@ -1690,34 +1690,34 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Oregon State</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>California</t>
+          <t>Syracuse</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>2.3</v>
+        <v>2.1</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Oregon State -3.0</t>
+          <t>Tennessee -13.5</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Oregon State -3</t>
+          <t>Tennessee -13.5</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Oregon State -5.3</t>
+          <t>Tennessee -15.6</t>
         </is>
       </c>
       <c r="H31" t="n">
-        <v>3</v>
+        <v>13.5</v>
       </c>
       <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr"/>
@@ -1731,34 +1731,34 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Texas A&amp;M</t>
+          <t>Southern Miss</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>UTSA</t>
+          <t>Mississippi State</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>2.100000000000001</v>
+        <v>2.1</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -21.5</t>
+          <t>Mississippi State -11.5</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -21.5</t>
+          <t>Mississippi State -11.5</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -19.4</t>
+          <t>Mississippi State -9.4</t>
         </is>
       </c>
       <c r="H32" t="n">
-        <v>21.5</v>
+        <v>-11.5</v>
       </c>
       <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr"/>
@@ -1772,12 +1772,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>North Carolina</t>
+          <t>Kentucky</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>TCU</t>
+          <t>Toledo</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1785,21 +1785,21 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>TCU -3.0</t>
+          <t>Kentucky -10.0</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>TCU -3</t>
+          <t>Kentucky -10</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>TCU -5.0</t>
+          <t>Kentucky -8.0</t>
         </is>
       </c>
       <c r="H33" t="n">
-        <v>-3</v>
+        <v>10</v>
       </c>
       <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr"/>
@@ -1813,34 +1813,34 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Tulane</t>
+          <t>Ohio State</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Northwestern</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Tulane -6.5</t>
+          <t>Ohio State -3.0</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Tulane -6.5</t>
+          <t>Ohio State -3</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Tulane -4.6</t>
+          <t>Ohio State -5.0</t>
         </is>
       </c>
       <c r="H34" t="n">
-        <v>6.5</v>
+        <v>3</v>
       </c>
       <c r="I34" t="inlineStr"/>
       <c r="J34" t="inlineStr"/>
@@ -1854,34 +1854,34 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Florida State</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Alabama</t>
+          <t>Notre Dame</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Alabama -13.5</t>
+          <t>Notre Dame -2.5</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Alabama -13.5</t>
+          <t>Notre Dame -2.5</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Alabama -15.4</t>
+          <t>Notre Dame -4.3</t>
         </is>
       </c>
       <c r="H35" t="n">
-        <v>-13.5</v>
+        <v>-2.5</v>
       </c>
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr"/>
@@ -1895,34 +1895,34 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Kansas</t>
+          <t>NC State</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Fresno State</t>
+          <t>East Carolina</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>1.800000000000001</v>
+        <v>1.699999999999999</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Kansas -14.0</t>
+          <t>NC State -12.5</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Kansas -14</t>
+          <t>NC State -12.5</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Kansas -12.2</t>
+          <t>NC State -14.2</t>
         </is>
       </c>
       <c r="H36" t="n">
-        <v>14</v>
+        <v>12.5</v>
       </c>
       <c r="I36" t="inlineStr"/>
       <c r="J36" t="inlineStr"/>
@@ -1936,34 +1936,34 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Kansas State</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Iowa State</t>
+          <t>New Mexico</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>1.8</v>
+        <v>1.600000000000001</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Kansas State -3.5</t>
+          <t>Michigan -36.5</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Kansas State -3.5</t>
+          <t>Michigan -36.5</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Kansas State -1.7</t>
+          <t>Michigan -38.1</t>
         </is>
       </c>
       <c r="H37" t="n">
-        <v>3.5</v>
+        <v>36.5</v>
       </c>
       <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr"/>
@@ -1977,34 +1977,34 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Cincinnati</t>
+          <t>Rutgers</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Nebraska</t>
+          <t>Ohio</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>1.7</v>
+        <v>1.4</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Nebraska -6.5</t>
+          <t>Rutgers -11.5</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Nebraska -6.5</t>
+          <t>Rutgers -11.5</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Nebraska -4.8</t>
+          <t>Rutgers -10.1</t>
         </is>
       </c>
       <c r="H38" t="n">
-        <v>-6.5</v>
+        <v>11.5</v>
       </c>
       <c r="I38" t="inlineStr"/>
       <c r="J38" t="inlineStr"/>
@@ -2018,34 +2018,34 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Fresno State</t>
+          <t>Wake Forest</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Georgia Southern</t>
+          <t>Kennesaw State</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1.2</v>
+        <v>1.399999999999999</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Fresno State -2.5</t>
+          <t>Wake Forest -17.5</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Fresno State -2.5</t>
+          <t>Wake Forest -17.5</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Fresno State -3.7</t>
+          <t>Wake Forest -18.9</t>
         </is>
       </c>
       <c r="H39" t="n">
-        <v>2.5</v>
+        <v>17.5</v>
       </c>
       <c r="I39" t="inlineStr"/>
       <c r="J39" t="inlineStr"/>
@@ -2059,12 +2059,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Clemson</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Notre Dame</t>
+          <t>LSU</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -2072,21 +2072,21 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Notre Dame -2.5</t>
+          <t>Clemson -3.5</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Notre Dame -2.5</t>
+          <t>Clemson -3.5</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Notre Dame -3.5</t>
+          <t>Clemson -4.5</t>
         </is>
       </c>
       <c r="H40" t="n">
-        <v>-2.5</v>
+        <v>3.5</v>
       </c>
       <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr"/>
@@ -2100,30 +2100,30 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Purdue</t>
+          <t>Minnesota</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Ball State</t>
+          <t>Buffalo</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.8999999999999986</v>
+        <v>0.6000000000000014</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Purdue -16.5</t>
+          <t>Minnesota -16.5</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Purdue -16.5</t>
+          <t>Minnesota -16.5</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Purdue -17.4</t>
+          <t>Minnesota -17.1</t>
         </is>
       </c>
       <c r="H41" t="n">
@@ -2141,30 +2141,30 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Purdue</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Ball State</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.6999999999999993</v>
+        <v>0.6000000000000014</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Minnesota -16.5</t>
+          <t>Purdue -16.5</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Minnesota -16.5</t>
+          <t>Purdue -16.5</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Minnesota -15.8</t>
+          <t>Purdue -17.1</t>
         </is>
       </c>
       <c r="H42" t="n">
@@ -2182,34 +2182,34 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Syracuse</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Tennessee</t>
+          <t>Georgia Tech</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.6999999999999993</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Tennessee -13.5</t>
+          <t>Georgia Tech -4.0</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Tennessee -13.5</t>
+          <t>Georgia Tech -4</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Tennessee -14.2</t>
+          <t>Georgia Tech -3.4</t>
         </is>
       </c>
       <c r="H43" t="n">
-        <v>-13.5</v>
+        <v>-4</v>
       </c>
       <c r="I43" t="inlineStr"/>
       <c r="J43" t="inlineStr"/>
@@ -2223,34 +2223,34 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Southern Miss</t>
+          <t>Kansas</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Mississippi State</t>
+          <t>Fresno State</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.5999999999999996</v>
+        <v>0.4000000000000004</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Mississippi State -11.5</t>
+          <t>Kansas -14.0</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Mississippi State -11.5</t>
+          <t>Kansas -14</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Mississippi State -10.9</t>
+          <t>Kansas -13.6</t>
         </is>
       </c>
       <c r="H44" t="n">
-        <v>-11.5</v>
+        <v>14</v>
       </c>
       <c r="I44" t="inlineStr"/>
       <c r="J44" t="inlineStr"/>
@@ -2264,34 +2264,34 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Ohio State</t>
+          <t>North Carolina</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>TCU</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.5</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Ohio State -3.0</t>
+          <t>TCU -3.0</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Ohio State -3</t>
+          <t>TCU -3</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Ohio State -3.5</t>
+          <t>TCU -2.6</t>
         </is>
       </c>
       <c r="H45" t="n">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="I45" t="inlineStr"/>
       <c r="J45" t="inlineStr"/>
@@ -2305,34 +2305,34 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Clemson</t>
+          <t>Tulane</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>LSU</t>
+          <t>Northwestern</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.3999999999999999</v>
+        <v>0.2999999999999998</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Clemson -3.5</t>
+          <t>Tulane -6.5</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Clemson -3.5</t>
+          <t>Tulane -6.5</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Clemson -3.1</t>
+          <t>Tulane -6.8</t>
         </is>
       </c>
       <c r="H46" t="n">
-        <v>3.5</v>
+        <v>6.5</v>
       </c>
       <c r="I46" t="inlineStr"/>
       <c r="J46" t="inlineStr"/>
@@ -2346,34 +2346,34 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Michigan</t>
+          <t>Fresno State</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>New Mexico</t>
+          <t>Georgia Southern</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.3999999999999986</v>
+        <v>0.2999999999999998</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Michigan -36.5</t>
+          <t>Fresno State -2.5</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Michigan -36.5</t>
+          <t>Fresno State -2.5</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Michigan -36.9</t>
+          <t>Fresno State -2.2</t>
         </is>
       </c>
       <c r="H47" t="n">
-        <v>36.5</v>
+        <v>2.5</v>
       </c>
       <c r="I47" t="inlineStr"/>
       <c r="J47" t="inlineStr"/>
@@ -2387,34 +2387,34 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Rutgers</t>
+          <t>Kansas State</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Ohio</t>
+          <t>Iowa State</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.09999999999999964</v>
+        <v>0.2000000000000002</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Rutgers -11.5</t>
+          <t>Kansas State -3.5</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Rutgers -11.5</t>
+          <t>Kansas State -3.5</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Rutgers -11.6</t>
+          <t>Kansas State -3.7</t>
         </is>
       </c>
       <c r="H48" t="n">
-        <v>11.5</v>
+        <v>3.5</v>
       </c>
       <c r="I48" t="inlineStr"/>
       <c r="J48" t="inlineStr"/>
@@ -2428,32 +2428,32 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>USC</t>
+          <t>Oklahoma State</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Missouri State</t>
+          <t>UT Martin</t>
         </is>
       </c>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr">
         <is>
-          <t>USC -34.5</t>
+          <t>Oklahoma State -22.5</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>USC -34.5</t>
+          <t>Oklahoma State -22.5</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>USC nan</t>
+          <t>Oklahoma State nan</t>
         </is>
       </c>
       <c r="H49" t="n">
-        <v>34.5</v>
+        <v>22.5</v>
       </c>
       <c r="I49" t="inlineStr"/>
       <c r="J49" t="inlineStr"/>
@@ -2461,6 +2461,747 @@
       <c r="L49" t="inlineStr"/>
       <c r="M49" t="inlineStr"/>
     </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Duke</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Elon</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Duke -33.5</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Duke -33.5</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Duke nan</t>
+        </is>
+      </c>
+      <c r="H50" t="n">
+        <v>33.5</v>
+      </c>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr"/>
+      <c r="K50" t="inlineStr"/>
+      <c r="L50" t="inlineStr"/>
+      <c r="M50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Houston</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Stephen F. Austin</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Houston -22.5</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Houston -22.5</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Houston nan</t>
+        </is>
+      </c>
+      <c r="H51" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="I51" t="inlineStr"/>
+      <c r="J51" t="inlineStr"/>
+      <c r="K51" t="inlineStr"/>
+      <c r="L51" t="inlineStr"/>
+      <c r="M51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>San Diego State</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Stony Brook</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>San Diego State -16.0</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>San Diego State -16</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>San Diego State nan</t>
+        </is>
+      </c>
+      <c r="H52" t="n">
+        <v>16</v>
+      </c>
+      <c r="I52" t="inlineStr"/>
+      <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr"/>
+      <c r="L52" t="inlineStr"/>
+      <c r="M52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Illinois</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Western Illinois</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Illinois -45.5</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Illinois -45.5</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Illinois nan</t>
+        </is>
+      </c>
+      <c r="H53" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="I53" t="inlineStr"/>
+      <c r="J53" t="inlineStr"/>
+      <c r="K53" t="inlineStr"/>
+      <c r="L53" t="inlineStr"/>
+      <c r="M53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Iowa State</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>South Dakota</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Iowa State -15.5</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Iowa State -15.5</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Iowa State nan</t>
+        </is>
+      </c>
+      <c r="H54" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr"/>
+      <c r="L54" t="inlineStr"/>
+      <c r="M54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Liberty</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Maine</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Liberty -25.5</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Liberty -25.5</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Liberty nan</t>
+        </is>
+      </c>
+      <c r="H55" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="I55" t="inlineStr"/>
+      <c r="J55" t="inlineStr"/>
+      <c r="K55" t="inlineStr"/>
+      <c r="L55" t="inlineStr"/>
+      <c r="M55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Oregon</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Montana State</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr"/>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Oregon -27.5</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Oregon -29.5</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Oregon nan</t>
+        </is>
+      </c>
+      <c r="H56" t="n">
+        <v>29.5</v>
+      </c>
+      <c r="I56" t="inlineStr"/>
+      <c r="J56" t="inlineStr"/>
+      <c r="K56" t="inlineStr"/>
+      <c r="L56" t="inlineStr"/>
+      <c r="M56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Oklahoma</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Illinois State</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Oklahoma -35.5</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Oklahoma -35.5</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Oklahoma nan</t>
+        </is>
+      </c>
+      <c r="H57" t="n">
+        <v>35.5</v>
+      </c>
+      <c r="I57" t="inlineStr"/>
+      <c r="J57" t="inlineStr"/>
+      <c r="K57" t="inlineStr"/>
+      <c r="L57" t="inlineStr"/>
+      <c r="M57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Iowa</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>UAlbany</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr"/>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Iowa -37.5</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Iowa -37.5</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Iowa nan</t>
+        </is>
+      </c>
+      <c r="H58" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="I58" t="inlineStr"/>
+      <c r="J58" t="inlineStr"/>
+      <c r="K58" t="inlineStr"/>
+      <c r="L58" t="inlineStr"/>
+      <c r="M58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>James Madison</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Weber State</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr"/>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>James Madison -25.5</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>James Madison -25.5</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>James Madison nan</t>
+        </is>
+      </c>
+      <c r="H59" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="I59" t="inlineStr"/>
+      <c r="J59" t="inlineStr"/>
+      <c r="K59" t="inlineStr"/>
+      <c r="L59" t="inlineStr"/>
+      <c r="M59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Arkansas State</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Southeast Missouri State</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr"/>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Arkansas State -10.5</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Arkansas State -10.5</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Arkansas State nan</t>
+        </is>
+      </c>
+      <c r="H60" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="I60" t="inlineStr"/>
+      <c r="J60" t="inlineStr"/>
+      <c r="K60" t="inlineStr"/>
+      <c r="L60" t="inlineStr"/>
+      <c r="M60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Troy</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Nicholls</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr"/>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Troy -22.5</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Troy -22.5</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Troy nan</t>
+        </is>
+      </c>
+      <c r="H61" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="I61" t="inlineStr"/>
+      <c r="J61" t="inlineStr"/>
+      <c r="K61" t="inlineStr"/>
+      <c r="L61" t="inlineStr"/>
+      <c r="M61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Vanderbilt</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Charleston Southern</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Vanderbilt -36.0</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Vanderbilt -36</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Vanderbilt nan</t>
+        </is>
+      </c>
+      <c r="H62" t="n">
+        <v>36</v>
+      </c>
+      <c r="I62" t="inlineStr"/>
+      <c r="J62" t="inlineStr"/>
+      <c r="K62" t="inlineStr"/>
+      <c r="L62" t="inlineStr"/>
+      <c r="M62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>USC</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Missouri State</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>USC -34.5</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>USC -34.5</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>USC nan</t>
+        </is>
+      </c>
+      <c r="H63" t="n">
+        <v>34.5</v>
+      </c>
+      <c r="I63" t="inlineStr"/>
+      <c r="J63" t="inlineStr"/>
+      <c r="K63" t="inlineStr"/>
+      <c r="L63" t="inlineStr"/>
+      <c r="M63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Louisiana Tech</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>SE Louisiana</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr"/>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Louisiana Tech -13.5</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Louisiana Tech -13.5</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Louisiana Tech nan</t>
+        </is>
+      </c>
+      <c r="H64" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="I64" t="inlineStr"/>
+      <c r="J64" t="inlineStr"/>
+      <c r="K64" t="inlineStr"/>
+      <c r="L64" t="inlineStr"/>
+      <c r="M64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>BYU</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Portland State</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr"/>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>BYU -34.5</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>BYU -35</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>BYU nan</t>
+        </is>
+      </c>
+      <c r="H65" t="n">
+        <v>35</v>
+      </c>
+      <c r="I65" t="inlineStr"/>
+      <c r="J65" t="inlineStr"/>
+      <c r="K65" t="inlineStr"/>
+      <c r="L65" t="inlineStr"/>
+      <c r="M65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>New Mexico State</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Bryant</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr"/>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>New Mexico State -19.5</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>New Mexico State -19.5</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>New Mexico State nan</t>
+        </is>
+      </c>
+      <c r="H66" t="n">
+        <v>19.5</v>
+      </c>
+      <c r="I66" t="inlineStr"/>
+      <c r="J66" t="inlineStr"/>
+      <c r="K66" t="inlineStr"/>
+      <c r="L66" t="inlineStr"/>
+      <c r="M66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Washington State</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Idaho</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr"/>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Washington State -9.5</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Washington State -9.5</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Washington State nan</t>
+        </is>
+      </c>
+      <c r="H67" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="I67" t="inlineStr"/>
+      <c r="J67" t="inlineStr"/>
+      <c r="K67" t="inlineStr"/>
+      <c r="L67" t="inlineStr"/>
+      <c r="M67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Arizona State</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Northern Arizona</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr"/>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Arizona State -28.5</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Arizona State -28.5</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Arizona State nan</t>
+        </is>
+      </c>
+      <c r="H68" t="n">
+        <v>28.5</v>
+      </c>
+      <c r="I68" t="inlineStr"/>
+      <c r="J68" t="inlineStr"/>
+      <c r="K68" t="inlineStr"/>
+      <c r="L68" t="inlineStr"/>
+      <c r="M68" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
updating to include raw pear on website
</commit_message>
<xml_diff>
--- a/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week1.xlsx
+++ b/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M48"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,30 +466,35 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>pr_spread</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>spread</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>actual_margin</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>actual_spread</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>PEAR ATS OPEN</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>PEAR ATS CLOSE</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>PEAR SU</t>
         </is>
@@ -528,13 +533,16 @@
         </is>
       </c>
       <c r="H2" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="I2" t="n">
         <v>-13.5</v>
       </c>
-      <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -569,13 +577,16 @@
         </is>
       </c>
       <c r="H3" t="n">
+        <v>23.7</v>
+      </c>
+      <c r="I3" t="n">
         <v>38.5</v>
       </c>
-      <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -610,13 +621,16 @@
         </is>
       </c>
       <c r="H4" t="n">
+        <v>-2.2</v>
+      </c>
+      <c r="I4" t="n">
         <v>12.5</v>
       </c>
-      <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -651,13 +665,16 @@
         </is>
       </c>
       <c r="H5" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="I5" t="n">
         <v>18.5</v>
       </c>
-      <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -692,13 +709,16 @@
         </is>
       </c>
       <c r="H6" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I6" t="n">
         <v>-8.5</v>
       </c>
-      <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -733,13 +753,16 @@
         </is>
       </c>
       <c r="H7" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="I7" t="n">
         <v>-1.5</v>
       </c>
-      <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -774,13 +797,16 @@
         </is>
       </c>
       <c r="H8" t="n">
+        <v>21.7</v>
+      </c>
+      <c r="I8" t="n">
         <v>14</v>
       </c>
-      <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -815,13 +841,16 @@
         </is>
       </c>
       <c r="H9" t="n">
+        <v>11.2</v>
+      </c>
+      <c r="I9" t="n">
         <v>3.5</v>
       </c>
-      <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -856,13 +885,16 @@
         </is>
       </c>
       <c r="H10" t="n">
+        <v>21.2</v>
+      </c>
+      <c r="I10" t="n">
         <v>13.5</v>
       </c>
-      <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -897,13 +929,16 @@
         </is>
       </c>
       <c r="H11" t="n">
+        <v>16</v>
+      </c>
+      <c r="I11" t="n">
         <v>23.5</v>
       </c>
-      <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -938,13 +973,16 @@
         </is>
       </c>
       <c r="H12" t="n">
+        <v>10.4</v>
+      </c>
+      <c r="I12" t="n">
         <v>17.5</v>
       </c>
-      <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -979,13 +1017,16 @@
         </is>
       </c>
       <c r="H13" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="I13" t="n">
         <v>9.5</v>
       </c>
-      <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1020,13 +1061,16 @@
         </is>
       </c>
       <c r="H14" t="n">
+        <v>17.4</v>
+      </c>
+      <c r="I14" t="n">
         <v>11.5</v>
       </c>
-      <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1061,13 +1105,16 @@
         </is>
       </c>
       <c r="H15" t="n">
+        <v>11</v>
+      </c>
+      <c r="I15" t="n">
         <v>16.5</v>
       </c>
-      <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1102,13 +1149,16 @@
         </is>
       </c>
       <c r="H16" t="n">
+        <v>40.7</v>
+      </c>
+      <c r="I16" t="n">
         <v>45.5</v>
       </c>
-      <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1116,40 +1166,43 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Oregon State</t>
+          <t>USC</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>California</t>
+          <t>Missouri State</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>4.2</v>
+        <v>4.399999999999999</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Oregon State -3.0</t>
+          <t>USC -34.5</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Oregon State -3</t>
+          <t>USC -34.5</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Oregon State -7.2</t>
+          <t>USC -30.1</t>
         </is>
       </c>
       <c r="H17" t="n">
-        <v>3</v>
-      </c>
-      <c r="I17" t="inlineStr"/>
+        <v>30.1</v>
+      </c>
+      <c r="I17" t="n">
+        <v>34.5</v>
+      </c>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1157,40 +1210,43 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Oregon State</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>App State</t>
+          <t>California</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>4.1</v>
+        <v>4.2</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>App State -8.5</t>
+          <t>Oregon State -3.0</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>App State -8.5</t>
+          <t>Oregon State -3</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>App State -12.6</t>
+          <t>Oregon State -7.2</t>
         </is>
       </c>
       <c r="H18" t="n">
-        <v>-8.5</v>
-      </c>
-      <c r="I18" t="inlineStr"/>
+        <v>7.2</v>
+      </c>
+      <c r="I18" t="n">
+        <v>3</v>
+      </c>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1198,40 +1254,43 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Massachusetts</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Temple</t>
+          <t>App State</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>4</v>
+        <v>4.1</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Temple -3.0</t>
+          <t>App State -8.5</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Temple -3</t>
+          <t>App State -8.5</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Massachusetts -1.0</t>
+          <t>App State -12.6</t>
         </is>
       </c>
       <c r="H19" t="n">
-        <v>-3</v>
-      </c>
-      <c r="I19" t="inlineStr"/>
+        <v>-12.6</v>
+      </c>
+      <c r="I19" t="n">
+        <v>-8.5</v>
+      </c>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1239,12 +1298,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Hawai'i</t>
+          <t>Massachusetts</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Stanford</t>
+          <t>Temple</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -1252,27 +1311,30 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Hawai'i -1.5</t>
+          <t>Temple -3.0</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Hawai'i -1.5</t>
+          <t>Temple -3</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Stanford -2.5</t>
+          <t>Massachusetts -1.0</t>
         </is>
       </c>
       <c r="H20" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="I20" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="I20" t="n">
+        <v>-3</v>
+      </c>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1280,40 +1342,43 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Akron</t>
+          <t>Hawai'i</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Wyoming</t>
+          <t>Stanford</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>3.9</v>
+        <v>4</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Wyoming -8.5</t>
+          <t>Hawai'i -1.5</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Wyoming -8.5</t>
+          <t>Hawai'i -1.5</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Wyoming -4.6</t>
+          <t>Stanford -2.5</t>
         </is>
       </c>
       <c r="H21" t="n">
-        <v>-8.5</v>
-      </c>
-      <c r="I21" t="inlineStr"/>
+        <v>-2.5</v>
+      </c>
+      <c r="I21" t="n">
+        <v>1.5</v>
+      </c>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1321,40 +1386,43 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Louisiana</t>
+          <t>Akron</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Rice</t>
+          <t>Wyoming</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>3.800000000000001</v>
+        <v>3.9</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Louisiana -14.5</t>
+          <t>Wyoming -8.5</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Louisiana -14.5</t>
+          <t>Wyoming -8.5</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Louisiana -10.7</t>
+          <t>Wyoming -4.6</t>
         </is>
       </c>
       <c r="H22" t="n">
-        <v>14.5</v>
-      </c>
-      <c r="I22" t="inlineStr"/>
+        <v>-4.6</v>
+      </c>
+      <c r="I22" t="n">
+        <v>-8.5</v>
+      </c>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1362,40 +1430,43 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Louisiana</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Colorado State</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>3.600000000000001</v>
+        <v>3.800000000000001</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Washington -20.5</t>
+          <t>Louisiana -14.5</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Washington -20.5</t>
+          <t>Louisiana -14.5</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Washington -16.9</t>
+          <t>Louisiana -10.7</t>
         </is>
       </c>
       <c r="H23" t="n">
-        <v>20.5</v>
-      </c>
-      <c r="I23" t="inlineStr"/>
+        <v>10.7</v>
+      </c>
+      <c r="I23" t="n">
+        <v>14.5</v>
+      </c>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1403,40 +1474,43 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Maryland</t>
+          <t>Washington</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Florida Atlantic</t>
+          <t>Colorado State</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>3.5</v>
+        <v>3.600000000000001</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Maryland -16.5</t>
+          <t>Washington -20.5</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Maryland -16.5</t>
+          <t>Washington -20.5</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Maryland -13.0</t>
+          <t>Washington -16.9</t>
         </is>
       </c>
       <c r="H24" t="n">
-        <v>16.5</v>
-      </c>
-      <c r="I24" t="inlineStr"/>
+        <v>16.9</v>
+      </c>
+      <c r="I24" t="n">
+        <v>20.5</v>
+      </c>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1444,12 +1518,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Texas A&amp;M</t>
+          <t>Maryland</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>UTSA</t>
+          <t>Florida Atlantic</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1457,27 +1531,30 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -21.5</t>
+          <t>Maryland -16.5</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -21.5</t>
+          <t>Maryland -16.5</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -25.0</t>
+          <t>Maryland -13.0</t>
         </is>
       </c>
       <c r="H25" t="n">
-        <v>21.5</v>
-      </c>
-      <c r="I25" t="inlineStr"/>
+        <v>13</v>
+      </c>
+      <c r="I25" t="n">
+        <v>16.5</v>
+      </c>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1485,40 +1562,43 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>Texas A&amp;M</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Marshall</t>
+          <t>UTSA</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>3.399999999999999</v>
+        <v>3.5</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Georgia -39.5</t>
+          <t>Texas A&amp;M -21.5</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Georgia -39.5</t>
+          <t>Texas A&amp;M -21.5</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Georgia -36.1</t>
+          <t>Texas A&amp;M -25.0</t>
         </is>
       </c>
       <c r="H26" t="n">
-        <v>39.5</v>
-      </c>
-      <c r="I26" t="inlineStr"/>
+        <v>25</v>
+      </c>
+      <c r="I26" t="n">
+        <v>21.5</v>
+      </c>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1526,40 +1606,43 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Florida State</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Alabama</t>
+          <t>Marshall</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>3.100000000000001</v>
+        <v>3.399999999999999</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Alabama -13.5</t>
+          <t>Georgia -39.5</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Alabama -13.5</t>
+          <t>Georgia -39.5</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Alabama -16.6</t>
+          <t>Georgia -36.1</t>
         </is>
       </c>
       <c r="H27" t="n">
-        <v>-13.5</v>
-      </c>
-      <c r="I27" t="inlineStr"/>
+        <v>36.1</v>
+      </c>
+      <c r="I27" t="n">
+        <v>39.5</v>
+      </c>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr"/>
       <c r="M27" t="inlineStr"/>
+      <c r="N27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1567,40 +1650,43 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>UCLA</t>
+          <t>Florida State</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>Alabama</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>3</v>
+        <v>3.100000000000001</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Utah -6.5</t>
+          <t>Alabama -13.5</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Utah -6.5</t>
+          <t>Alabama -13.5</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Utah -3.5</t>
+          <t>Alabama -16.6</t>
         </is>
       </c>
       <c r="H28" t="n">
-        <v>-6.5</v>
-      </c>
-      <c r="I28" t="inlineStr"/>
+        <v>-16.6</v>
+      </c>
+      <c r="I28" t="n">
+        <v>-13.5</v>
+      </c>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
       <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1608,40 +1694,43 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>South Carolina</t>
+          <t>UCLA</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Virginia Tech</t>
+          <t>Utah</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>South Carolina -8.5</t>
+          <t>Utah -6.5</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>South Carolina -8.5</t>
+          <t>Utah -6.5</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>South Carolina -5.7</t>
+          <t>Utah -3.5</t>
         </is>
       </c>
       <c r="H29" t="n">
-        <v>8.5</v>
-      </c>
-      <c r="I29" t="inlineStr"/>
+        <v>-3.5</v>
+      </c>
+      <c r="I29" t="n">
+        <v>-6.5</v>
+      </c>
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1649,40 +1738,43 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Cincinnati</t>
+          <t>South Carolina</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Nebraska</t>
+          <t>Virginia Tech</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>2.7</v>
+        <v>2.8</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Nebraska -6.5</t>
+          <t>South Carolina -8.5</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Nebraska -6.5</t>
+          <t>South Carolina -8.5</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Nebraska -3.8</t>
+          <t>South Carolina -5.7</t>
         </is>
       </c>
       <c r="H30" t="n">
-        <v>-6.5</v>
-      </c>
-      <c r="I30" t="inlineStr"/>
+        <v>5.7</v>
+      </c>
+      <c r="I30" t="n">
+        <v>8.5</v>
+      </c>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr"/>
       <c r="M30" t="inlineStr"/>
+      <c r="N30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1690,40 +1782,43 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Tennessee</t>
+          <t>Cincinnati</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Syracuse</t>
+          <t>Nebraska</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>2.1</v>
+        <v>2.7</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Tennessee -13.5</t>
+          <t>Nebraska -6.5</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Tennessee -13.5</t>
+          <t>Nebraska -6.5</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Tennessee -15.6</t>
+          <t>Nebraska -3.8</t>
         </is>
       </c>
       <c r="H31" t="n">
-        <v>13.5</v>
-      </c>
-      <c r="I31" t="inlineStr"/>
+        <v>-3.8</v>
+      </c>
+      <c r="I31" t="n">
+        <v>-6.5</v>
+      </c>
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr"/>
       <c r="M31" t="inlineStr"/>
+      <c r="N31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1731,12 +1826,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Southern Miss</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Mississippi State</t>
+          <t>Syracuse</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1744,27 +1839,30 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Mississippi State -11.5</t>
+          <t>Tennessee -13.5</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Mississippi State -11.5</t>
+          <t>Tennessee -13.5</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Mississippi State -9.4</t>
+          <t>Tennessee -15.6</t>
         </is>
       </c>
       <c r="H32" t="n">
-        <v>-11.5</v>
-      </c>
-      <c r="I32" t="inlineStr"/>
+        <v>15.6</v>
+      </c>
+      <c r="I32" t="n">
+        <v>13.5</v>
+      </c>
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr"/>
       <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1772,40 +1870,43 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Kentucky</t>
+          <t>Southern Miss</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Toledo</t>
+          <t>Mississippi State</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Kentucky -10.0</t>
+          <t>Mississippi State -11.5</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Kentucky -10</t>
+          <t>Mississippi State -11.5</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Kentucky -8.0</t>
+          <t>Mississippi State -9.4</t>
         </is>
       </c>
       <c r="H33" t="n">
-        <v>10</v>
-      </c>
-      <c r="I33" t="inlineStr"/>
+        <v>-9.4</v>
+      </c>
+      <c r="I33" t="n">
+        <v>-11.5</v>
+      </c>
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr"/>
       <c r="M33" t="inlineStr"/>
+      <c r="N33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1813,12 +1914,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Ohio State</t>
+          <t>Kentucky</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Toledo</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1826,27 +1927,30 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Ohio State -3.0</t>
+          <t>Kentucky -10.0</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Ohio State -3</t>
+          <t>Kentucky -10</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Ohio State -5.0</t>
+          <t>Kentucky -8.0</t>
         </is>
       </c>
       <c r="H34" t="n">
-        <v>3</v>
-      </c>
-      <c r="I34" t="inlineStr"/>
+        <v>8</v>
+      </c>
+      <c r="I34" t="n">
+        <v>10</v>
+      </c>
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr"/>
       <c r="M34" t="inlineStr"/>
+      <c r="N34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1854,40 +1958,43 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Ohio State</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Notre Dame</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Notre Dame -2.5</t>
+          <t>Ohio State -3.0</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Notre Dame -2.5</t>
+          <t>Ohio State -3</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Notre Dame -4.3</t>
+          <t>Ohio State -5.0</t>
         </is>
       </c>
       <c r="H35" t="n">
-        <v>-2.5</v>
-      </c>
-      <c r="I35" t="inlineStr"/>
+        <v>5</v>
+      </c>
+      <c r="I35" t="n">
+        <v>3</v>
+      </c>
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
       <c r="M35" t="inlineStr"/>
+      <c r="N35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1895,40 +2002,43 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>NC State</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>East Carolina</t>
+          <t>Notre Dame</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>1.699999999999999</v>
+        <v>1.8</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>NC State -12.5</t>
+          <t>Notre Dame -2.5</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>NC State -12.5</t>
+          <t>Notre Dame -2.5</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>NC State -14.2</t>
+          <t>Notre Dame -4.3</t>
         </is>
       </c>
       <c r="H36" t="n">
-        <v>12.5</v>
-      </c>
-      <c r="I36" t="inlineStr"/>
+        <v>-4.3</v>
+      </c>
+      <c r="I36" t="n">
+        <v>-2.5</v>
+      </c>
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
       <c r="M36" t="inlineStr"/>
+      <c r="N36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1936,40 +2046,43 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Michigan</t>
+          <t>NC State</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>New Mexico</t>
+          <t>East Carolina</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>1.600000000000001</v>
+        <v>1.699999999999999</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Michigan -36.5</t>
+          <t>NC State -12.5</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Michigan -36.5</t>
+          <t>NC State -12.5</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Michigan -38.1</t>
+          <t>NC State -14.2</t>
         </is>
       </c>
       <c r="H37" t="n">
-        <v>36.5</v>
-      </c>
-      <c r="I37" t="inlineStr"/>
+        <v>14.2</v>
+      </c>
+      <c r="I37" t="n">
+        <v>12.5</v>
+      </c>
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr"/>
       <c r="M37" t="inlineStr"/>
+      <c r="N37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1977,40 +2090,43 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Rutgers</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Ohio</t>
+          <t>New Mexico</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>1.4</v>
+        <v>1.600000000000001</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Rutgers -11.5</t>
+          <t>Michigan -36.5</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Rutgers -11.5</t>
+          <t>Michigan -36.5</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Rutgers -10.1</t>
+          <t>Michigan -38.1</t>
         </is>
       </c>
       <c r="H38" t="n">
-        <v>11.5</v>
-      </c>
-      <c r="I38" t="inlineStr"/>
+        <v>38.1</v>
+      </c>
+      <c r="I38" t="n">
+        <v>36.5</v>
+      </c>
       <c r="J38" t="inlineStr"/>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr"/>
       <c r="M38" t="inlineStr"/>
+      <c r="N38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -2018,40 +2134,43 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Wake Forest</t>
+          <t>Rutgers</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Kennesaw State</t>
+          <t>Ohio</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1.399999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Wake Forest -17.5</t>
+          <t>Rutgers -11.5</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Wake Forest -17.5</t>
+          <t>Rutgers -11.5</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Wake Forest -18.9</t>
+          <t>Rutgers -10.1</t>
         </is>
       </c>
       <c r="H39" t="n">
-        <v>17.5</v>
-      </c>
-      <c r="I39" t="inlineStr"/>
+        <v>10.1</v>
+      </c>
+      <c r="I39" t="n">
+        <v>11.5</v>
+      </c>
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
       <c r="M39" t="inlineStr"/>
+      <c r="N39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -2059,40 +2178,43 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Clemson</t>
+          <t>Wake Forest</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>LSU</t>
+          <t>Kennesaw State</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>1</v>
+        <v>1.399999999999999</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Clemson -3.5</t>
+          <t>Wake Forest -17.5</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Clemson -3.5</t>
+          <t>Wake Forest -17.5</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Clemson -4.5</t>
+          <t>Wake Forest -18.9</t>
         </is>
       </c>
       <c r="H40" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="I40" t="inlineStr"/>
+        <v>18.9</v>
+      </c>
+      <c r="I40" t="n">
+        <v>17.5</v>
+      </c>
       <c r="J40" t="inlineStr"/>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
       <c r="M40" t="inlineStr"/>
+      <c r="N40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -2100,40 +2222,43 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Clemson</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>LSU</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.6000000000000014</v>
+        <v>1</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Minnesota -16.5</t>
+          <t>Clemson -3.5</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Minnesota -16.5</t>
+          <t>Clemson -3.5</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Minnesota -17.1</t>
+          <t>Clemson -4.5</t>
         </is>
       </c>
       <c r="H41" t="n">
-        <v>16.5</v>
-      </c>
-      <c r="I41" t="inlineStr"/>
+        <v>4.5</v>
+      </c>
+      <c r="I41" t="n">
+        <v>3.5</v>
+      </c>
       <c r="J41" t="inlineStr"/>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr"/>
       <c r="M41" t="inlineStr"/>
+      <c r="N41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -2141,12 +2266,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Purdue</t>
+          <t>Minnesota</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Ball State</t>
+          <t>Buffalo</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -2154,27 +2279,30 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Purdue -16.5</t>
+          <t>Minnesota -16.5</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Purdue -16.5</t>
+          <t>Minnesota -16.5</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Purdue -17.1</t>
+          <t>Minnesota -17.1</t>
         </is>
       </c>
       <c r="H42" t="n">
+        <v>17.1</v>
+      </c>
+      <c r="I42" t="n">
         <v>16.5</v>
       </c>
-      <c r="I42" t="inlineStr"/>
       <c r="J42" t="inlineStr"/>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr"/>
       <c r="M42" t="inlineStr"/>
+      <c r="N42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -2182,40 +2310,43 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Colorado</t>
+          <t>Purdue</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Georgia Tech</t>
+          <t>Ball State</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.6000000000000001</v>
+        <v>0.6000000000000014</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Georgia Tech -4.0</t>
+          <t>Purdue -16.5</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Georgia Tech -4</t>
+          <t>Purdue -16.5</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Georgia Tech -3.4</t>
+          <t>Purdue -17.1</t>
         </is>
       </c>
       <c r="H43" t="n">
-        <v>-4</v>
-      </c>
-      <c r="I43" t="inlineStr"/>
+        <v>17.1</v>
+      </c>
+      <c r="I43" t="n">
+        <v>16.5</v>
+      </c>
       <c r="J43" t="inlineStr"/>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr"/>
       <c r="M43" t="inlineStr"/>
+      <c r="N43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -2223,40 +2354,43 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Kansas</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Fresno State</t>
+          <t>Georgia Tech</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.4000000000000004</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Kansas -14.0</t>
+          <t>Georgia Tech -4.0</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Kansas -14</t>
+          <t>Georgia Tech -4</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Kansas -13.6</t>
+          <t>Georgia Tech -3.4</t>
         </is>
       </c>
       <c r="H44" t="n">
-        <v>14</v>
-      </c>
-      <c r="I44" t="inlineStr"/>
+        <v>-3.4</v>
+      </c>
+      <c r="I44" t="n">
+        <v>-4</v>
+      </c>
       <c r="J44" t="inlineStr"/>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr"/>
       <c r="M44" t="inlineStr"/>
+      <c r="N44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -2264,40 +2398,43 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>North Carolina</t>
+          <t>Kansas</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>TCU</t>
+          <t>Fresno State</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.3999999999999999</v>
+        <v>0.4000000000000004</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>TCU -3.0</t>
+          <t>Kansas -14.0</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>TCU -3</t>
+          <t>Kansas -14</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>TCU -2.6</t>
+          <t>Kansas -13.6</t>
         </is>
       </c>
       <c r="H45" t="n">
-        <v>-3</v>
-      </c>
-      <c r="I45" t="inlineStr"/>
+        <v>13.6</v>
+      </c>
+      <c r="I45" t="n">
+        <v>14</v>
+      </c>
       <c r="J45" t="inlineStr"/>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr"/>
       <c r="M45" t="inlineStr"/>
+      <c r="N45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -2305,40 +2442,43 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Tulane</t>
+          <t>North Carolina</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Northwestern</t>
+          <t>TCU</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.2999999999999998</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Tulane -6.5</t>
+          <t>TCU -3.0</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Tulane -6.5</t>
+          <t>TCU -3</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Tulane -6.8</t>
+          <t>TCU -2.6</t>
         </is>
       </c>
       <c r="H46" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="I46" t="inlineStr"/>
+        <v>-2.6</v>
+      </c>
+      <c r="I46" t="n">
+        <v>-3</v>
+      </c>
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr"/>
       <c r="M46" t="inlineStr"/>
+      <c r="N46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -2346,12 +2486,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Fresno State</t>
+          <t>Tulane</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Georgia Southern</t>
+          <t>Northwestern</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -2359,27 +2499,30 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Fresno State -2.5</t>
+          <t>Tulane -6.5</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Fresno State -2.5</t>
+          <t>Tulane -6.5</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Fresno State -2.2</t>
+          <t>Tulane -6.8</t>
         </is>
       </c>
       <c r="H47" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="I47" t="inlineStr"/>
+        <v>6.8</v>
+      </c>
+      <c r="I47" t="n">
+        <v>6.5</v>
+      </c>
       <c r="J47" t="inlineStr"/>
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr"/>
       <c r="M47" t="inlineStr"/>
+      <c r="N47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -2387,40 +2530,87 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Kansas State</t>
+          <t>Fresno State</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Iowa State</t>
+          <t>Georgia Southern</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.2000000000000002</v>
+        <v>0.2999999999999998</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Kansas State -3.5</t>
+          <t>Fresno State -2.5</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Kansas State -3.5</t>
+          <t>Fresno State -2.5</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Kansas State -3.7</t>
+          <t>Fresno State -2.2</t>
         </is>
       </c>
       <c r="H48" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="I48" t="inlineStr"/>
+        <v>2.2</v>
+      </c>
+      <c r="I48" t="n">
+        <v>2.5</v>
+      </c>
       <c r="J48" t="inlineStr"/>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr"/>
       <c r="M48" t="inlineStr"/>
+      <c r="N48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Kansas State</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Iowa State</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0.2000000000000002</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Kansas State -3.5</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Kansas State -3.5</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Kansas State -3.7</t>
+        </is>
+      </c>
+      <c r="H49" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="I49" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="J49" t="inlineStr"/>
+      <c r="K49" t="inlineStr"/>
+      <c r="L49" t="inlineStr"/>
+      <c r="M49" t="inlineStr"/>
+      <c r="N49" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updating the spreads tracker
</commit_message>
<xml_diff>
--- a/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week1.xlsx
+++ b/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week1.xlsx
@@ -511,46 +511,58 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sam Houston</t>
+          <t>Ole Miss</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>UNLV</t>
+          <t>Georgia State</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>6.8</v>
+        <v>5.5</v>
       </c>
       <c r="E2" t="n">
-        <v>15.2</v>
+        <v>13.7</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>UNLV -13.5</t>
+          <t>Ole Miss -38.5</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>UNLV -13.5</t>
+          <t>Ole Miss -38.5</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Sam Houston -1.7</t>
+          <t>Ole Miss -24.8</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>1.7</v>
+        <v>24.8</v>
       </c>
       <c r="J2" t="n">
-        <v>-13.5</v>
-      </c>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
+        <v>38.5</v>
+      </c>
+      <c r="K2" t="n">
+        <v>56</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Ole Miss -56</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -558,46 +570,58 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Ole Miss</t>
+          <t>South Florida</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Georgia State</t>
+          <t>Boise State</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>5.5</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="E3" t="n">
-        <v>14.8</v>
+        <v>9.4</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Ole Miss -38.5</t>
+          <t>Boise State -8.5</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Ole Miss -38.5</t>
+          <t>Boise State -8.5</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Ole Miss -23.7</t>
+          <t>South Florida -0.9</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>23.7</v>
+        <v>0.9</v>
       </c>
       <c r="J3" t="n">
-        <v>38.5</v>
-      </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
+        <v>-8.5</v>
+      </c>
+      <c r="K3" t="n">
+        <v>27</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>South Florida -27</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -605,46 +629,58 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Virginia</t>
+          <t>Texas State</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Coastal Carolina</t>
+          <t>Eastern Michigan</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>6.8</v>
+        <v>3.9</v>
       </c>
       <c r="E4" t="n">
-        <v>14.7</v>
+        <v>8.600000000000001</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Virginia -12.5</t>
+          <t>Texas State -14.0</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Virginia -12.5</t>
+          <t>Texas State -14</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Coastal Carolina -2.2</t>
+          <t>Texas State -22.6</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>-2.2</v>
+        <v>22.6</v>
       </c>
       <c r="J4" t="n">
-        <v>12.5</v>
-      </c>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
+        <v>14</v>
+      </c>
+      <c r="K4" t="n">
+        <v>25</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Texas State -25</t>
+        </is>
+      </c>
+      <c r="M4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -652,46 +688,58 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Michigan State</t>
+          <t>Arizona</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Western Michigan</t>
+          <t>Hawai'i</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>7.8</v>
+        <v>3.9</v>
       </c>
       <c r="E5" t="n">
-        <v>11.1</v>
+        <v>8.5</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Michigan State -18.5</t>
+          <t>Arizona -13.5</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Michigan State -18.5</t>
+          <t>Arizona -13.5</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Michigan State -7.4</t>
+          <t>Arizona -22.0</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>7.4</v>
+        <v>22</v>
       </c>
       <c r="J5" t="n">
-        <v>18.5</v>
-      </c>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
+        <v>13.5</v>
+      </c>
+      <c r="K5" t="n">
+        <v>34</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Arizona -34</t>
+        </is>
+      </c>
+      <c r="M5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -699,46 +747,58 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>South Florida</t>
+          <t>Utah State</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Boise State</t>
+          <t>UTEP</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>8.699999999999999</v>
+        <v>5.4</v>
       </c>
       <c r="E6" t="n">
-        <v>9.1</v>
+        <v>7.9</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Boise State -8.5</t>
+          <t>Utah State -3.5</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Boise State -8.5</t>
+          <t>Utah State -3.5</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>South Florida -0.6</t>
+          <t>Utah State -11.4</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>0.6</v>
+        <v>11.4</v>
       </c>
       <c r="J6" t="n">
-        <v>-8.5</v>
-      </c>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
+        <v>3.5</v>
+      </c>
+      <c r="K6" t="n">
+        <v>12</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Utah State -12</t>
+        </is>
+      </c>
+      <c r="M6" t="n">
+        <v>1</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -755,10 +815,10 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>9.199999999999999</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="E7" t="n">
-        <v>7.7</v>
+        <v>7.6</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -772,20 +832,32 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Baylor -6.2</t>
+          <t>Baylor -6.1</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>6.2</v>
+        <v>6.1</v>
       </c>
       <c r="J7" t="n">
         <v>-1.5</v>
       </c>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
+      <c r="K7" t="n">
+        <v>-14</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Auburn -14</t>
+        </is>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -793,46 +865,58 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Texas State</t>
+          <t>Virginia</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Eastern Michigan</t>
+          <t>Coastal Carolina</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>4</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="E8" t="n">
-        <v>7.699999999999999</v>
+        <v>7.1</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Texas State -14.0</t>
+          <t>Virginia -12.5</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Texas State -14</t>
+          <t>Virginia -12.5</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Texas State -21.7</t>
+          <t>Virginia -5.4</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>21.7</v>
+        <v>5.4</v>
       </c>
       <c r="J8" t="n">
-        <v>14</v>
-      </c>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
+        <v>12.5</v>
+      </c>
+      <c r="K8" t="n">
+        <v>41</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Virginia -41</t>
+        </is>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -840,46 +924,58 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Utah State</t>
+          <t>Indiana</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>UTEP</t>
+          <t>Old Dominion</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>5.4</v>
+        <v>6.4</v>
       </c>
       <c r="E9" t="n">
-        <v>7.699999999999999</v>
+        <v>6.899999999999999</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Utah State -3.5</t>
+          <t>Indiana -23.5</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Utah State -3.5</t>
+          <t>Indiana -23.5</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Utah State -11.2</t>
+          <t>Indiana -16.6</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>11.2</v>
+        <v>16.6</v>
       </c>
       <c r="J9" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
+        <v>23.5</v>
+      </c>
+      <c r="K9" t="n">
+        <v>13</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Indiana -13</t>
+        </is>
+      </c>
+      <c r="M9" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" t="n">
+        <v>1</v>
+      </c>
+      <c r="O9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -887,46 +983,58 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Arizona</t>
+          <t>San José State</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Hawai'i</t>
+          <t>Central Michigan</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>4</v>
+        <v>3.9</v>
       </c>
       <c r="E10" t="n">
-        <v>7.699999999999999</v>
+        <v>6.600000000000001</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Arizona -13.5</t>
+          <t>San José State -11.5</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Arizona -13.5</t>
+          <t>San José State -11.5</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Arizona -21.2</t>
+          <t>San José State -18.1</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>21.2</v>
+        <v>18.1</v>
       </c>
       <c r="J10" t="n">
-        <v>13.5</v>
-      </c>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
+        <v>11.5</v>
+      </c>
+      <c r="K10" t="n">
+        <v>-2</v>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Central Michigan -2</t>
+        </is>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -934,46 +1042,58 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Wisconsin</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Old Dominion</t>
+          <t>Miami (OH)</t>
         </is>
       </c>
       <c r="D11" t="n">
+        <v>7.7</v>
+      </c>
+      <c r="E11" t="n">
         <v>6.4</v>
       </c>
-      <c r="E11" t="n">
-        <v>7.5</v>
-      </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Indiana -23.5</t>
+          <t>Wisconsin -17.5</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Indiana -23.5</t>
+          <t>Wisconsin -17.5</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Indiana -16.0</t>
+          <t>Wisconsin -11.1</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>16</v>
+        <v>11.1</v>
       </c>
       <c r="J11" t="n">
-        <v>23.5</v>
-      </c>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
+        <v>17.5</v>
+      </c>
+      <c r="K11" t="n">
+        <v>17</v>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Wisconsin -17</t>
+        </is>
+      </c>
+      <c r="M11" t="n">
+        <v>1</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1</v>
+      </c>
+      <c r="O11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -981,46 +1101,58 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Wisconsin</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Miami (OH)</t>
+          <t>App State</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>7.6</v>
+        <v>3</v>
       </c>
       <c r="E12" t="n">
-        <v>7.1</v>
+        <v>5</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Wisconsin -17.5</t>
+          <t>App State -8.5</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Wisconsin -17.5</t>
+          <t>App State -8.5</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Wisconsin -10.4</t>
+          <t>App State -13.5</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>10.4</v>
+        <v>-13.5</v>
       </c>
       <c r="J12" t="n">
-        <v>17.5</v>
-      </c>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
+        <v>-8.5</v>
+      </c>
+      <c r="K12" t="n">
+        <v>-23</v>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>App State -23</t>
+        </is>
+      </c>
+      <c r="M12" t="n">
+        <v>1</v>
+      </c>
+      <c r="N12" t="n">
+        <v>1</v>
+      </c>
+      <c r="O12" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1028,46 +1160,58 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Western Kentucky</t>
+          <t>Texas A&amp;M</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Sam Houston</t>
+          <t>UTSA</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>6.7</v>
+        <v>6.9</v>
       </c>
       <c r="E13" t="n">
-        <v>6.2</v>
+        <v>4.800000000000001</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Western Kentucky -9.5</t>
+          <t>Texas A&amp;M -21.5</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Western Kentucky -9.5</t>
+          <t>Texas A&amp;M -21.5</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Western Kentucky -3.3</t>
+          <t>Texas A&amp;M -26.3</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>3.3</v>
+        <v>26.3</v>
       </c>
       <c r="J13" t="n">
-        <v>9.5</v>
-      </c>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
+        <v>21.5</v>
+      </c>
+      <c r="K13" t="n">
+        <v>18</v>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Texas A&amp;M -18</t>
+        </is>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1075,46 +1219,58 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>San José State</t>
+          <t>UCF</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Central Michigan</t>
+          <t>Jacksonville State</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>4</v>
+        <v>7.5</v>
       </c>
       <c r="E14" t="n">
-        <v>5.899999999999999</v>
+        <v>4.800000000000001</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>San José State -11.5</t>
+          <t>UCF -16.5</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>San José State -11.5</t>
+          <t>UCF -16.5</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>San José State -17.4</t>
+          <t>UCF -11.7</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>17.4</v>
+        <v>11.7</v>
       </c>
       <c r="J14" t="n">
-        <v>11.5</v>
-      </c>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
+        <v>16.5</v>
+      </c>
+      <c r="K14" t="n">
+        <v>7</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>UCF -7</t>
+        </is>
+      </c>
+      <c r="M14" t="n">
+        <v>1</v>
+      </c>
+      <c r="N14" t="n">
+        <v>1</v>
+      </c>
+      <c r="O14" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1122,46 +1278,58 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>UCF</t>
+          <t>Hawai'i</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Jacksonville State</t>
+          <t>Stanford</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>7.4</v>
+        <v>4.8</v>
       </c>
       <c r="E15" t="n">
-        <v>5.5</v>
+        <v>4.6</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>UCF -16.5</t>
+          <t>Hawai'i -1.5</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>UCF -16.5</t>
+          <t>Hawai'i -1.5</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>UCF -11.0</t>
+          <t>Stanford -3.1</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>11</v>
+        <v>-3.1</v>
       </c>
       <c r="J15" t="n">
-        <v>16.5</v>
-      </c>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
+        <v>1.5</v>
+      </c>
+      <c r="K15" t="n">
+        <v>3</v>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Hawai'i -3</t>
+        </is>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1169,46 +1337,58 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Penn State</t>
+          <t>Florida State</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Nevada</t>
+          <t>Alabama</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>4.1</v>
+        <v>7.4</v>
       </c>
       <c r="E16" t="n">
-        <v>4.799999999999997</v>
+        <v>4.300000000000001</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Penn State -45.5</t>
+          <t>Alabama -13.5</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Penn State -45.5</t>
+          <t>Alabama -13.5</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Penn State -40.7</t>
+          <t>Alabama -17.8</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>40.7</v>
+        <v>-17.8</v>
       </c>
       <c r="J16" t="n">
-        <v>45.5</v>
-      </c>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
+        <v>-13.5</v>
+      </c>
+      <c r="K16" t="n">
+        <v>14</v>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Florida State -14</t>
+        </is>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1216,46 +1396,58 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>USC</t>
+          <t>Penn State</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Missouri State</t>
+          <t>Nevada</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>3.1</v>
+        <v>4.2</v>
       </c>
       <c r="E17" t="n">
-        <v>4.399999999999999</v>
+        <v>4.200000000000003</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>USC -34.5</t>
+          <t>Penn State -45.5</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>USC -34.5</t>
+          <t>Penn State -45.5</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>USC -30.1</t>
+          <t>Penn State -41.3</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>30.1</v>
+        <v>41.3</v>
       </c>
       <c r="J17" t="n">
-        <v>34.5</v>
-      </c>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr"/>
+        <v>45.5</v>
+      </c>
+      <c r="K17" t="n">
+        <v>35</v>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Penn State -35</t>
+        </is>
+      </c>
+      <c r="M17" t="n">
+        <v>1</v>
+      </c>
+      <c r="N17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O17" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1272,7 +1464,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>7.7</v>
+        <v>7.8</v>
       </c>
       <c r="E18" t="n">
         <v>4.2</v>
@@ -1298,11 +1490,23 @@
       <c r="J18" t="n">
         <v>3</v>
       </c>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr"/>
-      <c r="O18" t="inlineStr"/>
+      <c r="K18" t="n">
+        <v>-19</v>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>California -19</t>
+        </is>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1310,46 +1514,58 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Sam Houston</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>App State</t>
+          <t>UNLV</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>3.1</v>
+        <v>4.6</v>
       </c>
       <c r="E19" t="n">
-        <v>4.1</v>
+        <v>3.699999999999999</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>App State -8.5</t>
+          <t>UNLV -13.5</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>App State -8.5</t>
+          <t>UNLV -13.5</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>App State -12.6</t>
+          <t>UNLV -9.8</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>-12.6</v>
+        <v>-9.800000000000001</v>
       </c>
       <c r="J19" t="n">
-        <v>-8.5</v>
-      </c>
-      <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr"/>
-      <c r="O19" t="inlineStr"/>
+        <v>-13.5</v>
+      </c>
+      <c r="K19" t="n">
+        <v>-17</v>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>UNLV -17</t>
+        </is>
+      </c>
+      <c r="M19" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1357,46 +1573,58 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Massachusetts</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Temple</t>
+          <t>New Mexico</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>3.600000000000001</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Temple -3.0</t>
+          <t>Michigan -36.5</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Temple -3</t>
+          <t>Michigan -36.5</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Massachusetts -1.0</t>
+          <t>Michigan -40.1</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>1</v>
+        <v>40.1</v>
       </c>
       <c r="J20" t="n">
-        <v>-3</v>
-      </c>
-      <c r="K20" t="inlineStr"/>
-      <c r="L20" t="inlineStr"/>
-      <c r="M20" t="inlineStr"/>
-      <c r="N20" t="inlineStr"/>
-      <c r="O20" t="inlineStr"/>
+        <v>36.5</v>
+      </c>
+      <c r="K20" t="n">
+        <v>17</v>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Michigan -17</t>
+        </is>
+      </c>
+      <c r="M20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1404,46 +1632,58 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Hawai'i</t>
+          <t>Louisiana</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Stanford</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>4.8</v>
+        <v>6.9</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Hawai'i -1.5</t>
+          <t>Louisiana -14.5</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Hawai'i -1.5</t>
+          <t>Louisiana -14.5</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Stanford -2.5</t>
+          <t>Louisiana -10.9</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>-2.5</v>
+        <v>10.9</v>
       </c>
       <c r="J21" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr"/>
-      <c r="M21" t="inlineStr"/>
-      <c r="N21" t="inlineStr"/>
-      <c r="O21" t="inlineStr"/>
+        <v>14.5</v>
+      </c>
+      <c r="K21" t="n">
+        <v>-2</v>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Rice -2</t>
+        </is>
+      </c>
+      <c r="M21" t="n">
+        <v>1</v>
+      </c>
+      <c r="N21" t="n">
+        <v>1</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1463,7 +1703,7 @@
         <v>3.6</v>
       </c>
       <c r="E22" t="n">
-        <v>3.9</v>
+        <v>3.2</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -1477,20 +1717,32 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Wyoming -4.6</t>
+          <t>Wyoming -5.3</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>-4.6</v>
+        <v>-5.3</v>
       </c>
       <c r="J22" t="n">
         <v>-8.5</v>
       </c>
-      <c r="K22" t="inlineStr"/>
-      <c r="L22" t="inlineStr"/>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="inlineStr"/>
-      <c r="O22" t="inlineStr"/>
+      <c r="K22" t="n">
+        <v>-10</v>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Wyoming -10</t>
+        </is>
+      </c>
+      <c r="M22" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0</v>
+      </c>
+      <c r="O22" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1498,46 +1750,58 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Louisiana</t>
+          <t>Massachusetts</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Rice</t>
+          <t>Temple</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>6.8</v>
+        <v>5</v>
       </c>
       <c r="E23" t="n">
-        <v>3.800000000000001</v>
+        <v>3.1</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Louisiana -14.5</t>
+          <t>Temple -3.0</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Louisiana -14.5</t>
+          <t>Temple -3</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Louisiana -10.7</t>
+          <t>Massachusetts -0.1</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>10.7</v>
+        <v>0.1</v>
       </c>
       <c r="J23" t="n">
-        <v>14.5</v>
-      </c>
-      <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr"/>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr"/>
+        <v>-3</v>
+      </c>
+      <c r="K23" t="n">
+        <v>-32</v>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Temple -32</t>
+        </is>
+      </c>
+      <c r="M23" t="n">
+        <v>0</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1545,46 +1809,58 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Colorado State</t>
+          <t>Syracuse</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>6.2</v>
+        <v>7.2</v>
       </c>
       <c r="E24" t="n">
-        <v>3.600000000000001</v>
+        <v>3</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Washington -20.5</t>
+          <t>Tennessee -13.5</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Washington -20.5</t>
+          <t>Tennessee -13.5</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Washington -16.9</t>
+          <t>Tennessee -16.5</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>16.9</v>
+        <v>16.5</v>
       </c>
       <c r="J24" t="n">
-        <v>20.5</v>
-      </c>
-      <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr"/>
-      <c r="M24" t="inlineStr"/>
-      <c r="N24" t="inlineStr"/>
-      <c r="O24" t="inlineStr"/>
+        <v>13.5</v>
+      </c>
+      <c r="K24" t="n">
+        <v>19</v>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>Tennessee -19</t>
+        </is>
+      </c>
+      <c r="M24" t="n">
+        <v>1</v>
+      </c>
+      <c r="N24" t="n">
+        <v>1</v>
+      </c>
+      <c r="O24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1592,46 +1868,58 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Maryland</t>
+          <t>Washington</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Florida Atlantic</t>
+          <t>Colorado State</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>5.9</v>
+        <v>6.2</v>
       </c>
       <c r="E25" t="n">
-        <v>3.5</v>
+        <v>2.899999999999999</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Maryland -16.5</t>
+          <t>Washington -20.5</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Maryland -16.5</t>
+          <t>Washington -20.5</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Maryland -13.0</t>
+          <t>Washington -17.6</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>13</v>
+        <v>17.6</v>
       </c>
       <c r="J25" t="n">
-        <v>16.5</v>
-      </c>
-      <c r="K25" t="inlineStr"/>
-      <c r="L25" t="inlineStr"/>
-      <c r="M25" t="inlineStr"/>
-      <c r="N25" t="inlineStr"/>
-      <c r="O25" t="inlineStr"/>
+        <v>20.5</v>
+      </c>
+      <c r="K25" t="n">
+        <v>17</v>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>Washington -17</t>
+        </is>
+      </c>
+      <c r="M25" t="n">
+        <v>1</v>
+      </c>
+      <c r="N25" t="n">
+        <v>1</v>
+      </c>
+      <c r="O25" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1639,46 +1927,58 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Texas A&amp;M</t>
+          <t>UCLA</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>UTSA</t>
+          <t>Utah</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>6.9</v>
+        <v>7.8</v>
       </c>
       <c r="E26" t="n">
-        <v>3.5</v>
+        <v>2.7</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -21.5</t>
+          <t>Utah -6.5</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -21.5</t>
+          <t>Utah -6.5</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -25.0</t>
+          <t>Utah -3.8</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>25</v>
+        <v>-3.8</v>
       </c>
       <c r="J26" t="n">
-        <v>21.5</v>
-      </c>
-      <c r="K26" t="inlineStr"/>
-      <c r="L26" t="inlineStr"/>
-      <c r="M26" t="inlineStr"/>
-      <c r="N26" t="inlineStr"/>
-      <c r="O26" t="inlineStr"/>
+        <v>-6.5</v>
+      </c>
+      <c r="K26" t="n">
+        <v>-33</v>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>Utah -33</t>
+        </is>
+      </c>
+      <c r="M26" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0</v>
+      </c>
+      <c r="O26" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1686,46 +1986,58 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>USC</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Marshall</t>
+          <t>Missouri State</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>3.9</v>
+        <v>3</v>
       </c>
       <c r="E27" t="n">
-        <v>3.399999999999999</v>
+        <v>2.699999999999999</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Georgia -39.5</t>
+          <t>USC -34.5</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Georgia -39.5</t>
+          <t>USC -34.5</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Georgia -36.1</t>
+          <t>USC -31.8</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>36.1</v>
+        <v>31.8</v>
       </c>
       <c r="J27" t="n">
-        <v>39.5</v>
-      </c>
-      <c r="K27" t="inlineStr"/>
-      <c r="L27" t="inlineStr"/>
-      <c r="M27" t="inlineStr"/>
-      <c r="N27" t="inlineStr"/>
-      <c r="O27" t="inlineStr"/>
+        <v>34.5</v>
+      </c>
+      <c r="K27" t="n">
+        <v>60</v>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>USC -60</t>
+        </is>
+      </c>
+      <c r="M27" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0</v>
+      </c>
+      <c r="O27" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1733,46 +2045,58 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Florida State</t>
+          <t>Ohio State</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Alabama</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>7.4</v>
+        <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>3.100000000000001</v>
+        <v>2.3</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Alabama -13.5</t>
+          <t>Ohio State -3.0</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Alabama -13.5</t>
+          <t>Ohio State -3</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Alabama -16.6</t>
+          <t>Ohio State -5.3</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>-16.6</v>
+        <v>5.3</v>
       </c>
       <c r="J28" t="n">
-        <v>-13.5</v>
-      </c>
-      <c r="K28" t="inlineStr"/>
-      <c r="L28" t="inlineStr"/>
-      <c r="M28" t="inlineStr"/>
-      <c r="N28" t="inlineStr"/>
-      <c r="O28" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="K28" t="n">
+        <v>7</v>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>Ohio State -7</t>
+        </is>
+      </c>
+      <c r="M28" t="n">
+        <v>1</v>
+      </c>
+      <c r="N28" t="n">
+        <v>1</v>
+      </c>
+      <c r="O28" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1780,46 +2104,58 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>UCLA</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>Notre Dame</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>7.7</v>
+        <v>9.6</v>
       </c>
       <c r="E29" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Notre Dame -2.5</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Notre Dame -2.5</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Notre Dame -4.7</t>
+        </is>
+      </c>
+      <c r="I29" t="n">
+        <v>-4.7</v>
+      </c>
+      <c r="J29" t="n">
+        <v>-2.5</v>
+      </c>
+      <c r="K29" t="n">
         <v>3</v>
       </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>Utah -6.5</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>Utah -6.5</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>Utah -3.5</t>
-        </is>
-      </c>
-      <c r="I29" t="n">
-        <v>-3.5</v>
-      </c>
-      <c r="J29" t="n">
-        <v>-6.5</v>
-      </c>
-      <c r="K29" t="inlineStr"/>
-      <c r="L29" t="inlineStr"/>
-      <c r="M29" t="inlineStr"/>
-      <c r="N29" t="inlineStr"/>
-      <c r="O29" t="inlineStr"/>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>Miami -3</t>
+        </is>
+      </c>
+      <c r="M29" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0</v>
+      </c>
+      <c r="O29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1839,7 +2175,7 @@
         <v>9</v>
       </c>
       <c r="E30" t="n">
-        <v>2.8</v>
+        <v>2.1</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -1853,20 +2189,32 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>South Carolina -5.7</t>
+          <t>South Carolina -6.4</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>5.7</v>
+        <v>6.4</v>
       </c>
       <c r="J30" t="n">
         <v>8.5</v>
       </c>
-      <c r="K30" t="inlineStr"/>
-      <c r="L30" t="inlineStr"/>
-      <c r="M30" t="inlineStr"/>
-      <c r="N30" t="inlineStr"/>
-      <c r="O30" t="inlineStr"/>
+      <c r="K30" t="n">
+        <v>13</v>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>South Carolina -13</t>
+        </is>
+      </c>
+      <c r="M30" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1883,10 +2231,10 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>9</v>
+        <v>9.1</v>
       </c>
       <c r="E31" t="n">
-        <v>2.7</v>
+        <v>2.1</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -1900,20 +2248,32 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Nebraska -3.8</t>
+          <t>Nebraska -4.4</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>-3.8</v>
+        <v>-4.4</v>
       </c>
       <c r="J31" t="n">
         <v>-6.5</v>
       </c>
-      <c r="K31" t="inlineStr"/>
-      <c r="L31" t="inlineStr"/>
-      <c r="M31" t="inlineStr"/>
-      <c r="N31" t="inlineStr"/>
-      <c r="O31" t="inlineStr"/>
+      <c r="K31" t="n">
+        <v>-3</v>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>Nebraska -3</t>
+        </is>
+      </c>
+      <c r="M31" t="n">
+        <v>1</v>
+      </c>
+      <c r="N31" t="n">
+        <v>1</v>
+      </c>
+      <c r="O31" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1921,46 +2281,58 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Tennessee</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Syracuse</t>
+          <t>Marshall</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>7.2</v>
+        <v>4.2</v>
       </c>
       <c r="E32" t="n">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Tennessee -13.5</t>
+          <t>Georgia -39.5</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Tennessee -13.5</t>
+          <t>Georgia -39.5</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Tennessee -15.6</t>
+          <t>Georgia -37.5</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>15.6</v>
+        <v>37.5</v>
       </c>
       <c r="J32" t="n">
-        <v>13.5</v>
-      </c>
-      <c r="K32" t="inlineStr"/>
-      <c r="L32" t="inlineStr"/>
-      <c r="M32" t="inlineStr"/>
-      <c r="N32" t="inlineStr"/>
-      <c r="O32" t="inlineStr"/>
+        <v>39.5</v>
+      </c>
+      <c r="K32" t="n">
+        <v>38</v>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>Georgia -38</t>
+        </is>
+      </c>
+      <c r="M32" t="n">
+        <v>1</v>
+      </c>
+      <c r="N32" t="n">
+        <v>1</v>
+      </c>
+      <c r="O32" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1968,46 +2340,58 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Southern Miss</t>
+          <t>Kentucky</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Mississippi State</t>
+          <t>Toledo</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>4.7</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="E33" t="n">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Mississippi State -11.5</t>
+          <t>Kentucky -10.0</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Mississippi State -11.5</t>
+          <t>Kentucky -10</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Mississippi State -9.4</t>
+          <t>Kentucky -8.0</t>
         </is>
       </c>
       <c r="I33" t="n">
-        <v>-9.4</v>
+        <v>8</v>
       </c>
       <c r="J33" t="n">
-        <v>-11.5</v>
-      </c>
-      <c r="K33" t="inlineStr"/>
-      <c r="L33" t="inlineStr"/>
-      <c r="M33" t="inlineStr"/>
-      <c r="N33" t="inlineStr"/>
-      <c r="O33" t="inlineStr"/>
+        <v>10</v>
+      </c>
+      <c r="K33" t="n">
+        <v>8</v>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>Kentucky -8</t>
+        </is>
+      </c>
+      <c r="M33" t="n">
+        <v>1</v>
+      </c>
+      <c r="N33" t="n">
+        <v>1</v>
+      </c>
+      <c r="O33" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -2015,46 +2399,58 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Kentucky</t>
+          <t>Southern Miss</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Toledo</t>
+          <t>Mississippi State</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>8.199999999999999</v>
+        <v>4.9</v>
       </c>
       <c r="E34" t="n">
         <v>2</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Kentucky -10.0</t>
+          <t>Mississippi State -11.5</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Kentucky -10</t>
+          <t>Mississippi State -11.5</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Kentucky -8.0</t>
+          <t>Mississippi State -9.5</t>
         </is>
       </c>
       <c r="I34" t="n">
-        <v>8</v>
+        <v>-9.5</v>
       </c>
       <c r="J34" t="n">
-        <v>10</v>
-      </c>
-      <c r="K34" t="inlineStr"/>
-      <c r="L34" t="inlineStr"/>
-      <c r="M34" t="inlineStr"/>
-      <c r="N34" t="inlineStr"/>
-      <c r="O34" t="inlineStr"/>
+        <v>-11.5</v>
+      </c>
+      <c r="K34" t="n">
+        <v>-17</v>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>Mississippi State -17</t>
+        </is>
+      </c>
+      <c r="M34" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0</v>
+      </c>
+      <c r="O34" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -2062,46 +2458,58 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Ohio State</t>
+          <t>Tulane</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Northwestern</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>10</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Ohio State -3.0</t>
+          <t>Tulane -6.5</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Ohio State -3</t>
+          <t>Tulane -6.5</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Ohio State -5.0</t>
+          <t>Tulane -8.4</t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>5</v>
+        <v>8.4</v>
       </c>
       <c r="J35" t="n">
-        <v>3</v>
-      </c>
-      <c r="K35" t="inlineStr"/>
-      <c r="L35" t="inlineStr"/>
-      <c r="M35" t="inlineStr"/>
-      <c r="N35" t="inlineStr"/>
-      <c r="O35" t="inlineStr"/>
+        <v>6.5</v>
+      </c>
+      <c r="K35" t="n">
+        <v>20</v>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>Tulane -20</t>
+        </is>
+      </c>
+      <c r="M35" t="n">
+        <v>1</v>
+      </c>
+      <c r="N35" t="n">
+        <v>1</v>
+      </c>
+      <c r="O35" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -2109,46 +2517,58 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Michigan State</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Notre Dame</t>
+          <t>Western Michigan</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>9.5</v>
+        <v>5</v>
       </c>
       <c r="E36" t="n">
-        <v>1.8</v>
+        <v>1.800000000000001</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Notre Dame -2.5</t>
+          <t>Michigan State -18.5</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Notre Dame -2.5</t>
+          <t>Michigan State -18.5</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Notre Dame -4.3</t>
+          <t>Michigan State -16.7</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>-4.3</v>
+        <v>16.7</v>
       </c>
       <c r="J36" t="n">
-        <v>-2.5</v>
-      </c>
-      <c r="K36" t="inlineStr"/>
-      <c r="L36" t="inlineStr"/>
-      <c r="M36" t="inlineStr"/>
-      <c r="N36" t="inlineStr"/>
-      <c r="O36" t="inlineStr"/>
+        <v>18.5</v>
+      </c>
+      <c r="K36" t="n">
+        <v>17</v>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>Michigan State -17</t>
+        </is>
+      </c>
+      <c r="M36" t="n">
+        <v>1</v>
+      </c>
+      <c r="N36" t="n">
+        <v>1</v>
+      </c>
+      <c r="O36" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -2156,46 +2576,58 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>NC State</t>
+          <t>Purdue</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>East Carolina</t>
+          <t>Ball State</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>7.2</v>
+        <v>3.2</v>
       </c>
       <c r="E37" t="n">
-        <v>1.699999999999999</v>
+        <v>1.300000000000001</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>NC State -12.5</t>
+          <t>Purdue -16.5</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>NC State -12.5</t>
+          <t>Purdue -16.5</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>NC State -14.2</t>
+          <t>Purdue -17.8</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>14.2</v>
+        <v>17.8</v>
       </c>
       <c r="J37" t="n">
-        <v>12.5</v>
-      </c>
-      <c r="K37" t="inlineStr"/>
-      <c r="L37" t="inlineStr"/>
-      <c r="M37" t="inlineStr"/>
-      <c r="N37" t="inlineStr"/>
-      <c r="O37" t="inlineStr"/>
+        <v>16.5</v>
+      </c>
+      <c r="K37" t="n">
+        <v>31</v>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>Purdue -31</t>
+        </is>
+      </c>
+      <c r="M37" t="n">
+        <v>1</v>
+      </c>
+      <c r="N37" t="n">
+        <v>1</v>
+      </c>
+      <c r="O37" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -2203,46 +2635,58 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Michigan</t>
+          <t>Clemson</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>New Mexico</t>
+          <t>LSU</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>2.5</v>
+        <v>9.9</v>
       </c>
       <c r="E38" t="n">
-        <v>1.600000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Michigan -36.5</t>
+          <t>Clemson -3.5</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Michigan -36.5</t>
+          <t>Clemson -3.5</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Michigan -38.1</t>
+          <t>Clemson -4.7</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>38.1</v>
+        <v>4.7</v>
       </c>
       <c r="J38" t="n">
-        <v>36.5</v>
-      </c>
-      <c r="K38" t="inlineStr"/>
-      <c r="L38" t="inlineStr"/>
-      <c r="M38" t="inlineStr"/>
-      <c r="N38" t="inlineStr"/>
-      <c r="O38" t="inlineStr"/>
+        <v>3.5</v>
+      </c>
+      <c r="K38" t="n">
+        <v>-7</v>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>LSU -7</t>
+        </is>
+      </c>
+      <c r="M38" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" t="n">
+        <v>0</v>
+      </c>
+      <c r="O38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -2250,46 +2694,58 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Rutgers</t>
+          <t>Minnesota</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Ohio</t>
+          <t>Buffalo</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>7.9</v>
+        <v>5.8</v>
       </c>
       <c r="E39" t="n">
-        <v>1.4</v>
+        <v>1.199999999999999</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Rutgers -11.5</t>
+          <t>Minnesota -16.5</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Rutgers -11.5</t>
+          <t>Minnesota -16.5</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Rutgers -10.1</t>
+          <t>Minnesota -17.7</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>10.1</v>
+        <v>17.7</v>
       </c>
       <c r="J39" t="n">
-        <v>11.5</v>
-      </c>
-      <c r="K39" t="inlineStr"/>
-      <c r="L39" t="inlineStr"/>
-      <c r="M39" t="inlineStr"/>
-      <c r="N39" t="inlineStr"/>
-      <c r="O39" t="inlineStr"/>
+        <v>16.5</v>
+      </c>
+      <c r="K39" t="n">
+        <v>13</v>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>Minnesota -13</t>
+        </is>
+      </c>
+      <c r="M39" t="n">
+        <v>0</v>
+      </c>
+      <c r="N39" t="n">
+        <v>0</v>
+      </c>
+      <c r="O39" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -2306,10 +2762,10 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="E40" t="n">
-        <v>1.399999999999999</v>
+        <v>1.100000000000001</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -2323,20 +2779,32 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Wake Forest -18.9</t>
+          <t>Wake Forest -18.6</t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>18.9</v>
+        <v>18.6</v>
       </c>
       <c r="J40" t="n">
         <v>17.5</v>
       </c>
-      <c r="K40" t="inlineStr"/>
-      <c r="L40" t="inlineStr"/>
-      <c r="M40" t="inlineStr"/>
-      <c r="N40" t="inlineStr"/>
-      <c r="O40" t="inlineStr"/>
+      <c r="K40" t="n">
+        <v>1</v>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>Wake Forest -1</t>
+        </is>
+      </c>
+      <c r="M40" t="n">
+        <v>0</v>
+      </c>
+      <c r="N40" t="n">
+        <v>0</v>
+      </c>
+      <c r="O40" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -2344,46 +2812,58 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Clemson</t>
+          <t>Western Kentucky</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>LSU</t>
+          <t>Sam Houston</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>9.9</v>
+        <v>5</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>0.9000000000000004</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Clemson -3.5</t>
+          <t>Western Kentucky -9.5</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Clemson -3.5</t>
+          <t>Western Kentucky -9.5</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Clemson -4.5</t>
+          <t>Western Kentucky -10.4</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>4.5</v>
+        <v>10.4</v>
       </c>
       <c r="J41" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="K41" t="inlineStr"/>
-      <c r="L41" t="inlineStr"/>
-      <c r="M41" t="inlineStr"/>
-      <c r="N41" t="inlineStr"/>
-      <c r="O41" t="inlineStr"/>
+        <v>9.5</v>
+      </c>
+      <c r="K41" t="n">
+        <v>17</v>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>Western Kentucky -17</t>
+        </is>
+      </c>
+      <c r="M41" t="n">
+        <v>1</v>
+      </c>
+      <c r="N41" t="n">
+        <v>1</v>
+      </c>
+      <c r="O41" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -2391,46 +2871,58 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Rutgers</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Ohio</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>5.8</v>
+        <v>8</v>
       </c>
       <c r="E42" t="n">
-        <v>0.6000000000000014</v>
+        <v>0.9000000000000004</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Minnesota -16.5</t>
+          <t>Rutgers -11.5</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Minnesota -16.5</t>
+          <t>Rutgers -11.5</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Minnesota -17.1</t>
+          <t>Rutgers -10.6</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>17.1</v>
+        <v>10.6</v>
       </c>
       <c r="J42" t="n">
-        <v>16.5</v>
-      </c>
-      <c r="K42" t="inlineStr"/>
-      <c r="L42" t="inlineStr"/>
-      <c r="M42" t="inlineStr"/>
-      <c r="N42" t="inlineStr"/>
-      <c r="O42" t="inlineStr"/>
+        <v>11.5</v>
+      </c>
+      <c r="K42" t="n">
+        <v>3</v>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>Rutgers -3</t>
+        </is>
+      </c>
+      <c r="M42" t="n">
+        <v>1</v>
+      </c>
+      <c r="N42" t="n">
+        <v>1</v>
+      </c>
+      <c r="O42" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -2438,46 +2930,58 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Purdue</t>
+          <t>NC State</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Ball State</t>
+          <t>East Carolina</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>3.3</v>
+        <v>7.4</v>
       </c>
       <c r="E43" t="n">
-        <v>0.6000000000000014</v>
+        <v>0.6999999999999993</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Purdue -16.5</t>
+          <t>NC State -12.5</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Purdue -16.5</t>
+          <t>NC State -12.5</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Purdue -17.1</t>
+          <t>NC State -13.2</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>17.1</v>
+        <v>13.2</v>
       </c>
       <c r="J43" t="n">
-        <v>16.5</v>
-      </c>
-      <c r="K43" t="inlineStr"/>
-      <c r="L43" t="inlineStr"/>
-      <c r="M43" t="inlineStr"/>
-      <c r="N43" t="inlineStr"/>
-      <c r="O43" t="inlineStr"/>
+        <v>12.5</v>
+      </c>
+      <c r="K43" t="n">
+        <v>7</v>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>NC State -7</t>
+        </is>
+      </c>
+      <c r="M43" t="n">
+        <v>0</v>
+      </c>
+      <c r="N43" t="n">
+        <v>0</v>
+      </c>
+      <c r="O43" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -2485,46 +2989,58 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Colorado</t>
+          <t>North Carolina</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Georgia Tech</t>
+          <t>TCU</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>8.1</v>
+        <v>8.5</v>
       </c>
       <c r="E44" t="n">
-        <v>0.6000000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Georgia Tech -4.0</t>
+          <t>TCU -3.0</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Georgia Tech -4</t>
+          <t>TCU -3</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Georgia Tech -3.4</t>
+          <t>TCU -2.5</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>-3.4</v>
+        <v>-2.5</v>
       </c>
       <c r="J44" t="n">
-        <v>-4</v>
-      </c>
-      <c r="K44" t="inlineStr"/>
-      <c r="L44" t="inlineStr"/>
-      <c r="M44" t="inlineStr"/>
-      <c r="N44" t="inlineStr"/>
-      <c r="O44" t="inlineStr"/>
+        <v>-3</v>
+      </c>
+      <c r="K44" t="n">
+        <v>-34</v>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>TCU -34</t>
+        </is>
+      </c>
+      <c r="M44" t="n">
+        <v>0</v>
+      </c>
+      <c r="N44" t="n">
+        <v>0</v>
+      </c>
+      <c r="O44" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -2532,46 +3048,58 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Kansas</t>
+          <t>Kansas State</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Fresno State</t>
+          <t>Iowa State</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>6.8</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="E45" t="n">
-        <v>0.4000000000000004</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Kansas -14.0</t>
+          <t>Kansas State -3.5</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Kansas -14</t>
+          <t>Kansas State -3.5</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Kansas -13.6</t>
+          <t>Kansas State -3.9</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>13.6</v>
+        <v>3.9</v>
       </c>
       <c r="J45" t="n">
-        <v>14</v>
-      </c>
-      <c r="K45" t="inlineStr"/>
-      <c r="L45" t="inlineStr"/>
-      <c r="M45" t="inlineStr"/>
-      <c r="N45" t="inlineStr"/>
-      <c r="O45" t="inlineStr"/>
+        <v>3.5</v>
+      </c>
+      <c r="K45" t="n">
+        <v>-3</v>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>Iowa State -3</t>
+        </is>
+      </c>
+      <c r="M45" t="n">
+        <v>0</v>
+      </c>
+      <c r="N45" t="n">
+        <v>0</v>
+      </c>
+      <c r="O45" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -2579,46 +3107,58 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>North Carolina</t>
+          <t>Fresno State</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>TCU</t>
+          <t>Georgia Southern</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>8.4</v>
+        <v>7.5</v>
       </c>
       <c r="E46" t="n">
-        <v>0.3999999999999999</v>
+        <v>0.2000000000000002</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>TCU -3.0</t>
+          <t>Fresno State -2.5</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>TCU -3</t>
+          <t>Fresno State -2.5</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>TCU -2.6</t>
+          <t>Fresno State -2.3</t>
         </is>
       </c>
       <c r="I46" t="n">
-        <v>-2.6</v>
+        <v>2.3</v>
       </c>
       <c r="J46" t="n">
-        <v>-3</v>
-      </c>
-      <c r="K46" t="inlineStr"/>
-      <c r="L46" t="inlineStr"/>
-      <c r="M46" t="inlineStr"/>
-      <c r="N46" t="inlineStr"/>
-      <c r="O46" t="inlineStr"/>
+        <v>2.5</v>
+      </c>
+      <c r="K46" t="n">
+        <v>28</v>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>Fresno State -28</t>
+        </is>
+      </c>
+      <c r="M46" t="n">
+        <v>0</v>
+      </c>
+      <c r="N46" t="n">
+        <v>0</v>
+      </c>
+      <c r="O46" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -2626,46 +3166,58 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Tulane</t>
+          <t>Maryland</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Northwestern</t>
+          <t>Florida Atlantic</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>8.199999999999999</v>
+        <v>5.7</v>
       </c>
       <c r="E47" t="n">
-        <v>0.2999999999999998</v>
+        <v>0.1000000000000014</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Tulane -6.5</t>
+          <t>Maryland -16.5</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Tulane -6.5</t>
+          <t>Maryland -16.5</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Tulane -6.8</t>
+          <t>Maryland -16.4</t>
         </is>
       </c>
       <c r="I47" t="n">
-        <v>6.8</v>
+        <v>16.4</v>
       </c>
       <c r="J47" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="K47" t="inlineStr"/>
-      <c r="L47" t="inlineStr"/>
-      <c r="M47" t="inlineStr"/>
-      <c r="N47" t="inlineStr"/>
-      <c r="O47" t="inlineStr"/>
+        <v>16.5</v>
+      </c>
+      <c r="K47" t="n">
+        <v>32</v>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>Maryland -32</t>
+        </is>
+      </c>
+      <c r="M47" t="n">
+        <v>0</v>
+      </c>
+      <c r="N47" t="n">
+        <v>0</v>
+      </c>
+      <c r="O47" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -2673,46 +3225,58 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Fresno State</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Georgia Southern</t>
+          <t>Georgia Tech</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>7.4</v>
+        <v>8.1</v>
       </c>
       <c r="E48" t="n">
-        <v>0.2999999999999998</v>
+        <v>0.1000000000000001</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Fresno State -2.5</t>
+          <t>Georgia Tech -4.0</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Fresno State -2.5</t>
+          <t>Georgia Tech -4</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Fresno State -2.2</t>
+          <t>Georgia Tech -3.9</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>2.2</v>
+        <v>-3.9</v>
       </c>
       <c r="J48" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="K48" t="inlineStr"/>
-      <c r="L48" t="inlineStr"/>
-      <c r="M48" t="inlineStr"/>
-      <c r="N48" t="inlineStr"/>
-      <c r="O48" t="inlineStr"/>
+        <v>-4</v>
+      </c>
+      <c r="K48" t="n">
+        <v>-7</v>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>Georgia Tech -7</t>
+        </is>
+      </c>
+      <c r="M48" t="n">
+        <v>0</v>
+      </c>
+      <c r="N48" t="n">
+        <v>0</v>
+      </c>
+      <c r="O48" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -2720,46 +3284,58 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Kansas State</t>
+          <t>Kansas</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Iowa State</t>
+          <t>Fresno State</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>9.199999999999999</v>
+        <v>6.9</v>
       </c>
       <c r="E49" t="n">
-        <v>0.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Kansas State -3.5</t>
+          <t>Kansas -14.0</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Kansas State -3.5</t>
+          <t>Kansas -14</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Kansas State -3.7</t>
+          <t>Kansas -14.0</t>
         </is>
       </c>
       <c r="I49" t="n">
-        <v>3.7</v>
+        <v>14</v>
       </c>
       <c r="J49" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="K49" t="inlineStr"/>
-      <c r="L49" t="inlineStr"/>
-      <c r="M49" t="inlineStr"/>
-      <c r="N49" t="inlineStr"/>
-      <c r="O49" t="inlineStr"/>
+        <v>14</v>
+      </c>
+      <c r="K49" t="n">
+        <v>24</v>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>Kansas -24</t>
+        </is>
+      </c>
+      <c r="M49" t="n">
+        <v>1</v>
+      </c>
+      <c r="N49" t="n">
+        <v>1</v>
+      </c>
+      <c r="O49" t="n">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>